<commit_message>
ERR advance payment rule removal and RPN validation addition
</commit_message>
<xml_diff>
--- a/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
+++ b/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91288C5E-7BC8-4763-8F8E-10F76E516E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC6B4A-309D-4B0B-A7AF-D6D04101D463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="193">
   <si>
     <t xml:space="preserve">Latest Version History </t>
   </si>
@@ -604,12 +604,6 @@
     <t>77, 105, 4, 55, 65, 75, 116, 117, 118, 119, 121</t>
   </si>
   <si>
-    <t>Advance payment should not exceed 1000 or -1000 per claim</t>
-  </si>
-  <si>
-    <t>A maximum of 1000 per claim can be paid in respect of Advance Payments</t>
-  </si>
-  <si>
     <t>Advance payment reconciliation reported in error</t>
   </si>
   <si>
@@ -617,6 +611,24 @@
   </si>
   <si>
     <t xml:space="preserve">Advance Payment reconciliation </t>
+  </si>
+  <si>
+    <t>No record found for Employer Registration Id provided.</t>
+  </si>
+  <si>
+    <t>No record found for Employer Registration Id provided due to RPN service error.</t>
+  </si>
+  <si>
+    <t>EmployerRegistrationId</t>
+  </si>
+  <si>
+    <t>173, 174</t>
+  </si>
+  <si>
+    <t>Added rules</t>
+  </si>
+  <si>
+    <t>Removed 173</t>
   </si>
 </sst>
 </file>
@@ -967,7 +979,7 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1267,6 +1279,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -21968,7 +21983,7 @@
   <dimension ref="B8:E68"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22103,16 +22118,32 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="59"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="64"/>
+      <c r="B20" s="59">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="104">
+        <v>45371</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="21"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="63"/>
+      <c r="B21" s="21">
+        <v>0.15</v>
+      </c>
+      <c r="C21" s="71">
+        <v>173</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="E21" s="70">
+        <v>45373</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="21"/>
@@ -22416,7 +22447,7 @@
   <dimension ref="A1:BM342"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -24529,7 +24560,7 @@
     </row>
     <row r="46" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="82">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B46" s="83" t="s">
         <v>34</v>
@@ -24537,8 +24568,8 @@
       <c r="C46" s="84" t="s">
         <v>184</v>
       </c>
-      <c r="D46" s="82">
-        <v>19</v>
+      <c r="D46" s="82" t="s">
+        <v>36</v>
       </c>
       <c r="E46" s="85" t="s">
         <v>37</v>
@@ -24556,13 +24587,13 @@
         <v>81</v>
       </c>
       <c r="J46" s="82" t="s">
-        <v>117</v>
+        <v>40</v>
       </c>
       <c r="K46" s="82" t="s">
         <v>47</v>
       </c>
       <c r="L46" s="86">
-        <v>2612</v>
+        <v>2614</v>
       </c>
       <c r="M46" s="87" t="s">
         <v>185</v>
@@ -24571,105 +24602,106 @@
         <v>77</v>
       </c>
       <c r="O46" s="83" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="82">
-        <v>174</v>
-      </c>
-      <c r="B47" s="83" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="84" t="s">
         <v>186</v>
       </c>
-      <c r="D47" s="82" t="s">
+    </row>
+    <row r="47" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="101" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" s="102"/>
+      <c r="C47" s="102"/>
+      <c r="D47" s="102"/>
+      <c r="E47" s="102"/>
+      <c r="F47" s="102"/>
+      <c r="G47" s="102"/>
+      <c r="H47" s="102"/>
+      <c r="I47" s="102"/>
+      <c r="J47" s="102"/>
+      <c r="K47" s="102"/>
+      <c r="L47" s="102"/>
+      <c r="M47" s="102"/>
+      <c r="N47" s="102"/>
+      <c r="O47" s="103"/>
+      <c r="P47" s="13"/>
+    </row>
+    <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="98"/>
+      <c r="C48" s="98"/>
+      <c r="D48" s="98"/>
+      <c r="E48" s="98"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="98"/>
+      <c r="H48" s="98"/>
+      <c r="I48" s="98"/>
+      <c r="J48" s="98"/>
+      <c r="K48" s="98"/>
+      <c r="L48" s="98"/>
+      <c r="M48" s="98"/>
+      <c r="N48" s="98"/>
+      <c r="O48" s="99"/>
+      <c r="P48" s="13"/>
+    </row>
+    <row r="49" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="44">
+        <v>148</v>
+      </c>
+      <c r="B49" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="E47" s="85" t="s">
+      <c r="E49" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="F47" s="85" t="s">
+      <c r="F49" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="85">
-        <v>200</v>
-      </c>
-      <c r="H47" s="85" t="s">
-        <v>80</v>
-      </c>
-      <c r="I47" s="85" t="s">
-        <v>81</v>
-      </c>
-      <c r="J47" s="82" t="s">
+      <c r="G49" s="44">
+        <v>403</v>
+      </c>
+      <c r="H49" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J49" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="K47" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="L47" s="86">
-        <v>2614</v>
-      </c>
-      <c r="M47" s="87" t="s">
-        <v>187</v>
-      </c>
-      <c r="N47" s="83" t="s">
-        <v>77</v>
-      </c>
-      <c r="O47" s="83" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="101" t="s">
-        <v>143</v>
-      </c>
-      <c r="B48" s="102"/>
-      <c r="C48" s="102"/>
-      <c r="D48" s="102"/>
-      <c r="E48" s="102"/>
-      <c r="F48" s="102"/>
-      <c r="G48" s="102"/>
-      <c r="H48" s="102"/>
-      <c r="I48" s="102"/>
-      <c r="J48" s="102"/>
-      <c r="K48" s="102"/>
-      <c r="L48" s="102"/>
-      <c r="M48" s="102"/>
-      <c r="N48" s="102"/>
-      <c r="O48" s="103"/>
-      <c r="P48" s="13"/>
-    </row>
-    <row r="49" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="98"/>
-      <c r="C49" s="98"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="98"/>
-      <c r="G49" s="98"/>
-      <c r="H49" s="98"/>
-      <c r="I49" s="98"/>
-      <c r="J49" s="98"/>
-      <c r="K49" s="98"/>
-      <c r="L49" s="98"/>
-      <c r="M49" s="98"/>
-      <c r="N49" s="98"/>
-      <c r="O49" s="99"/>
+      <c r="K49" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="L49" s="44">
+        <v>1111</v>
+      </c>
+      <c r="M49" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="N49" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O49" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="P49" s="13"/>
     </row>
-    <row r="50" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B50" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C50" s="45" t="s">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="D50" s="44" t="s">
         <v>36</v>
@@ -24696,76 +24728,76 @@
         <v>41</v>
       </c>
       <c r="L50" s="44">
-        <v>1111</v>
+        <v>1016</v>
       </c>
       <c r="M50" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="N50" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O50" s="22" t="s">
-        <v>58</v>
+        <v>35</v>
+      </c>
+      <c r="N50" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O50" s="45" t="s">
+        <v>36</v>
       </c>
       <c r="P50" s="13"/>
     </row>
-    <row r="51" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="44">
-        <v>146</v>
+    <row r="51" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>52</v>
       </c>
       <c r="B51" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C51" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D51" s="44" t="s">
+      <c r="C51" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E51" s="44" t="s">
+      <c r="E51" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F51" s="44" t="s">
+      <c r="F51" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G51" s="44">
-        <v>403</v>
-      </c>
-      <c r="H51" s="44" t="s">
+      <c r="G51" s="16">
+        <v>401</v>
+      </c>
+      <c r="H51" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I51" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J51" s="44" t="s">
+      <c r="J51" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K51" s="44" t="s">
+      <c r="K51" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L51" s="44">
-        <v>1016</v>
-      </c>
-      <c r="M51" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="N51" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="O51" s="45" t="s">
+      <c r="L51" s="4">
+        <v>1012</v>
+      </c>
+      <c r="M51" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N51" s="23" t="s">
         <v>36</v>
       </c>
+      <c r="O51" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="P51" s="13"/>
     </row>
-    <row r="52" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B52" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C52" s="23" t="s">
-        <v>43</v>
+      <c r="C52" s="15" t="s">
+        <v>45</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>36</v>
@@ -24792,28 +24824,28 @@
         <v>41</v>
       </c>
       <c r="L52" s="4">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="M52" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N52" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O52" s="30" t="s">
+      <c r="O52" s="29" t="s">
         <v>36</v>
       </c>
       <c r="P52" s="13"/>
     </row>
-    <row r="53" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B53" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>36</v>
@@ -24825,7 +24857,7 @@
         <v>37</v>
       </c>
       <c r="G53" s="16">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="H53" s="35" t="s">
         <v>38</v>
@@ -24833,35 +24865,34 @@
       <c r="I53" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="J53" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K53" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L53" s="4">
-        <v>1013</v>
-      </c>
-      <c r="M53" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="N53" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O53" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="P53" s="13"/>
-    </row>
-    <row r="54" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K53" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="L53" s="16">
+        <v>1003</v>
+      </c>
+      <c r="M53" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="N53" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O53" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B54" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>36</v>
@@ -24873,7 +24904,7 @@
         <v>37</v>
       </c>
       <c r="G54" s="16">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H54" s="35" t="s">
         <v>38</v>
@@ -24885,13 +24916,13 @@
         <v>40</v>
       </c>
       <c r="K54" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L54" s="16">
-        <v>1003</v>
+        <v>51</v>
+      </c>
+      <c r="L54" s="17">
+        <v>1004</v>
       </c>
       <c r="M54" s="23" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="N54" s="22" t="s">
         <v>147</v>
@@ -24900,15 +24931,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B55" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>149</v>
+      <c r="C55" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>36</v>
@@ -24920,7 +24951,7 @@
         <v>37</v>
       </c>
       <c r="G55" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H55" s="35" t="s">
         <v>38</v>
@@ -24928,45 +24959,94 @@
       <c r="I55" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J55" s="16" t="s">
+      <c r="J55" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K55" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L55" s="17">
-        <v>1004</v>
-      </c>
-      <c r="M55" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="N55" s="22" t="s">
-        <v>147</v>
+      <c r="K55" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L55" s="5">
+        <v>1005</v>
+      </c>
+      <c r="M55" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="N55" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="O55" s="22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="14"/>
+      <c r="V55" s="14"/>
+      <c r="W55" s="14"/>
+      <c r="X55" s="14"/>
+      <c r="Y55" s="14"/>
+      <c r="Z55" s="14"/>
+      <c r="AA55" s="14"/>
+      <c r="AB55" s="14"/>
+      <c r="AC55" s="14"/>
+      <c r="AD55" s="14"/>
+      <c r="AE55" s="14"/>
+      <c r="AF55" s="14"/>
+      <c r="AG55" s="14"/>
+      <c r="AH55" s="14"/>
+      <c r="AI55" s="14"/>
+      <c r="AJ55" s="14"/>
+      <c r="AK55" s="14"/>
+      <c r="AL55" s="14"/>
+      <c r="AM55" s="14"/>
+      <c r="AN55" s="14"/>
+      <c r="AO55" s="14"/>
+      <c r="AP55" s="14"/>
+      <c r="AQ55" s="14"/>
+      <c r="AR55" s="14"/>
+      <c r="AS55" s="14"/>
+      <c r="AT55" s="14"/>
+      <c r="AU55" s="14"/>
+      <c r="AV55" s="14"/>
+      <c r="AW55" s="14"/>
+      <c r="AX55" s="14"/>
+      <c r="AY55" s="14"/>
+      <c r="AZ55" s="14"/>
+      <c r="BA55" s="14"/>
+      <c r="BB55" s="14"/>
+      <c r="BC55" s="14"/>
+      <c r="BD55" s="14"/>
+      <c r="BE55" s="14"/>
+      <c r="BF55" s="14"/>
+      <c r="BG55" s="14"/>
+      <c r="BH55" s="14"/>
+      <c r="BI55" s="14"/>
+      <c r="BJ55" s="14"/>
+      <c r="BK55" s="14"/>
+      <c r="BL55" s="14"/>
+      <c r="BM55" s="14"/>
+    </row>
+    <row r="56" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="B56" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56" s="4" t="s">
+      <c r="C56" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G56" s="16">
+      <c r="G56" s="4">
         <v>403</v>
       </c>
       <c r="H56" s="35" t="s">
@@ -24975,94 +25055,45 @@
       <c r="I56" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J56" s="4" t="s">
+      <c r="J56" s="54" t="s">
         <v>40</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L56" s="5">
-        <v>1005</v>
+        <v>51</v>
+      </c>
+      <c r="L56" s="54">
+        <v>1015</v>
       </c>
       <c r="M56" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="N56" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="N56" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O56" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q56" s="14"/>
-      <c r="R56" s="14"/>
-      <c r="S56" s="14"/>
-      <c r="T56" s="14"/>
-      <c r="U56" s="14"/>
-      <c r="V56" s="14"/>
-      <c r="W56" s="14"/>
-      <c r="X56" s="14"/>
-      <c r="Y56" s="14"/>
-      <c r="Z56" s="14"/>
-      <c r="AA56" s="14"/>
-      <c r="AB56" s="14"/>
-      <c r="AC56" s="14"/>
-      <c r="AD56" s="14"/>
-      <c r="AE56" s="14"/>
-      <c r="AF56" s="14"/>
-      <c r="AG56" s="14"/>
-      <c r="AH56" s="14"/>
-      <c r="AI56" s="14"/>
-      <c r="AJ56" s="14"/>
-      <c r="AK56" s="14"/>
-      <c r="AL56" s="14"/>
-      <c r="AM56" s="14"/>
-      <c r="AN56" s="14"/>
-      <c r="AO56" s="14"/>
-      <c r="AP56" s="14"/>
-      <c r="AQ56" s="14"/>
-      <c r="AR56" s="14"/>
-      <c r="AS56" s="14"/>
-      <c r="AT56" s="14"/>
-      <c r="AU56" s="14"/>
-      <c r="AV56" s="14"/>
-      <c r="AW56" s="14"/>
-      <c r="AX56" s="14"/>
-      <c r="AY56" s="14"/>
-      <c r="AZ56" s="14"/>
-      <c r="BA56" s="14"/>
-      <c r="BB56" s="14"/>
-      <c r="BC56" s="14"/>
-      <c r="BD56" s="14"/>
-      <c r="BE56" s="14"/>
-      <c r="BF56" s="14"/>
-      <c r="BG56" s="14"/>
-      <c r="BH56" s="14"/>
-      <c r="BI56" s="14"/>
-      <c r="BJ56" s="14"/>
-      <c r="BK56" s="14"/>
-      <c r="BL56" s="14"/>
-      <c r="BM56" s="14"/>
-    </row>
-    <row r="57" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="O56" s="55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="B57" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C57" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D57" s="54" t="s">
+      <c r="C57" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E57" s="54" t="s">
+      <c r="E57" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F57" s="54" t="s">
+      <c r="F57" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="16">
         <v>403</v>
       </c>
       <c r="H57" s="35" t="s">
@@ -25071,34 +25102,34 @@
       <c r="I57" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J57" s="54" t="s">
+      <c r="J57" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K57" s="4" t="s">
+      <c r="K57" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="L57" s="54">
-        <v>1015</v>
-      </c>
-      <c r="M57" s="22" t="s">
-        <v>55</v>
+      <c r="L57" s="17">
+        <v>1006</v>
+      </c>
+      <c r="M57" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="N57" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="O57" s="55" t="s">
-        <v>36</v>
+        <v>147</v>
+      </c>
+      <c r="O57" s="22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>36</v>
@@ -25122,13 +25153,13 @@
         <v>40</v>
       </c>
       <c r="K58" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L58" s="17">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="M58" s="23" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N58" s="22" t="s">
         <v>147</v>
@@ -25139,13 +25170,13 @@
     </row>
     <row r="59" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>36</v>
@@ -25172,10 +25203,10 @@
         <v>47</v>
       </c>
       <c r="L59" s="17">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="M59" s="23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="N59" s="22" t="s">
         <v>147</v>
@@ -25186,15 +25217,15 @@
     </row>
     <row r="60" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="D60" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E60" s="4" t="s">
@@ -25216,32 +25247,32 @@
         <v>40</v>
       </c>
       <c r="K60" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L60" s="17">
-        <v>1008</v>
+        <v>41</v>
+      </c>
+      <c r="L60" s="16">
+        <v>1011</v>
       </c>
       <c r="M60" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N60" s="22" t="s">
         <v>147</v>
       </c>
       <c r="O60" s="22" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" s="57" t="s">
         <v>144</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D61" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E61" s="4" t="s">
@@ -25251,7 +25282,7 @@
         <v>37</v>
       </c>
       <c r="G61" s="16">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H61" s="35" t="s">
         <v>38</v>
@@ -25259,121 +25290,122 @@
       <c r="I61" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J61" s="16" t="s">
+      <c r="J61" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K61" s="16" t="s">
+      <c r="K61" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L61" s="16">
-        <v>1011</v>
-      </c>
-      <c r="M61" s="23" t="s">
-        <v>64</v>
+      <c r="L61" s="4">
+        <v>2501</v>
+      </c>
+      <c r="M61" s="22" t="s">
+        <v>153</v>
       </c>
       <c r="N61" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="O61" s="22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="95" t="s">
+        <v>154</v>
+      </c>
+      <c r="B62" s="96"/>
+      <c r="C62" s="96"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="96"/>
+      <c r="F62" s="96"/>
+      <c r="G62" s="96"/>
+      <c r="H62" s="96"/>
+      <c r="I62" s="96"/>
+      <c r="J62" s="96"/>
+      <c r="K62" s="96"/>
+      <c r="L62" s="96"/>
+      <c r="M62" s="96"/>
+      <c r="N62" s="96"/>
+      <c r="O62" s="100"/>
+      <c r="P62" s="13"/>
+    </row>
+    <row r="63" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="98"/>
+      <c r="C63" s="98"/>
+      <c r="D63" s="98"/>
+      <c r="E63" s="98"/>
+      <c r="F63" s="98"/>
+      <c r="G63" s="98"/>
+      <c r="H63" s="98"/>
+      <c r="I63" s="98"/>
+      <c r="J63" s="98"/>
+      <c r="K63" s="98"/>
+      <c r="L63" s="98"/>
+      <c r="M63" s="98"/>
+      <c r="N63" s="98"/>
+      <c r="O63" s="99"/>
+      <c r="P63" s="13"/>
+    </row>
+    <row r="64" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="44">
+        <v>148</v>
+      </c>
+      <c r="B64" s="57" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D64" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F64" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G64" s="44">
+        <v>403</v>
+      </c>
+      <c r="H64" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="I64" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J64" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K64" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="L64" s="44">
+        <v>1111</v>
+      </c>
+      <c r="M64" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="N64" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="O61" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
-        <v>61</v>
-      </c>
-      <c r="B62" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G62" s="16">
-        <v>404</v>
-      </c>
-      <c r="H62" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="I62" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L62" s="4">
-        <v>2501</v>
-      </c>
-      <c r="M62" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="N62" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="O62" s="22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="95" t="s">
-        <v>154</v>
-      </c>
-      <c r="B63" s="96"/>
-      <c r="C63" s="96"/>
-      <c r="D63" s="96"/>
-      <c r="E63" s="96"/>
-      <c r="F63" s="96"/>
-      <c r="G63" s="96"/>
-      <c r="H63" s="96"/>
-      <c r="I63" s="96"/>
-      <c r="J63" s="96"/>
-      <c r="K63" s="96"/>
-      <c r="L63" s="96"/>
-      <c r="M63" s="96"/>
-      <c r="N63" s="96"/>
-      <c r="O63" s="100"/>
-      <c r="P63" s="13"/>
-    </row>
-    <row r="64" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="B64" s="98"/>
-      <c r="C64" s="98"/>
-      <c r="D64" s="98"/>
-      <c r="E64" s="98"/>
-      <c r="F64" s="98"/>
-      <c r="G64" s="98"/>
-      <c r="H64" s="98"/>
-      <c r="I64" s="98"/>
-      <c r="J64" s="98"/>
-      <c r="K64" s="98"/>
-      <c r="L64" s="98"/>
-      <c r="M64" s="98"/>
-      <c r="N64" s="98"/>
-      <c r="O64" s="99"/>
+      <c r="O64" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="P64" s="13"/>
     </row>
-    <row r="65" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="44">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B65" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="D65" s="44" t="s">
         <v>36</v>
@@ -25400,76 +25432,76 @@
         <v>41</v>
       </c>
       <c r="L65" s="44">
-        <v>1111</v>
+        <v>1016</v>
       </c>
       <c r="M65" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="N65" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O65" s="22" t="s">
-        <v>58</v>
+        <v>35</v>
+      </c>
+      <c r="N65" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O65" s="45" t="s">
+        <v>36</v>
       </c>
       <c r="P65" s="13"/>
     </row>
-    <row r="66" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="44">
-        <v>146</v>
+    <row r="66" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>62</v>
       </c>
       <c r="B66" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C66" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" s="44" t="s">
+      <c r="C66" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E66" s="44" t="s">
+      <c r="E66" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F66" s="44" t="s">
+      <c r="F66" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G66" s="44">
-        <v>403</v>
-      </c>
-      <c r="H66" s="44" t="s">
+      <c r="G66" s="16">
+        <v>401</v>
+      </c>
+      <c r="H66" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I66" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J66" s="44" t="s">
+      <c r="J66" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K66" s="44" t="s">
+      <c r="K66" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L66" s="44">
-        <v>1016</v>
-      </c>
-      <c r="M66" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="N66" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="O66" s="45" t="s">
+      <c r="L66" s="4">
+        <v>1012</v>
+      </c>
+      <c r="M66" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N66" s="23" t="s">
         <v>36</v>
       </c>
+      <c r="O66" s="30" t="s">
+        <v>36</v>
+      </c>
       <c r="P66" s="13"/>
     </row>
-    <row r="67" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B67" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>36</v>
@@ -25496,28 +25528,28 @@
         <v>41</v>
       </c>
       <c r="L67" s="4">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="M67" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N67" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O67" s="30" t="s">
+      <c r="O67" s="29" t="s">
         <v>36</v>
       </c>
       <c r="P67" s="13"/>
     </row>
-    <row r="68" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B68" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>36</v>
@@ -25529,7 +25561,7 @@
         <v>37</v>
       </c>
       <c r="G68" s="16">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="H68" s="35" t="s">
         <v>38</v>
@@ -25537,35 +25569,34 @@
       <c r="I68" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J68" s="4" t="s">
+      <c r="J68" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K68" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L68" s="4">
-        <v>1013</v>
-      </c>
-      <c r="M68" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="N68" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O68" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="P68" s="13"/>
-    </row>
-    <row r="69" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="K68" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="L68" s="17">
+        <v>1003</v>
+      </c>
+      <c r="M68" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="N68" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B69" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>36</v>
@@ -25577,7 +25608,7 @@
         <v>37</v>
       </c>
       <c r="G69" s="16">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H69" s="35" t="s">
         <v>38</v>
@@ -25585,34 +25616,34 @@
       <c r="I69" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J69" s="17" t="s">
+      <c r="J69" s="16" t="s">
         <v>40</v>
       </c>
       <c r="K69" s="16" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L69" s="17">
-        <v>1003</v>
-      </c>
-      <c r="M69" s="29" t="s">
-        <v>48</v>
+        <v>1004</v>
+      </c>
+      <c r="M69" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="N69" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="O69" s="4" t="s">
+      <c r="O69" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B70" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C70" s="15" t="s">
-        <v>149</v>
+      <c r="C70" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>36</v>
@@ -25624,7 +25655,7 @@
         <v>37</v>
       </c>
       <c r="G70" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H70" s="35" t="s">
         <v>38</v>
@@ -25632,45 +25663,94 @@
       <c r="I70" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J70" s="16" t="s">
+      <c r="J70" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K70" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L70" s="17">
-        <v>1004</v>
+      <c r="K70" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L70" s="5">
+        <v>1005</v>
       </c>
       <c r="M70" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="N70" s="22" t="s">
-        <v>147</v>
+        <v>54</v>
+      </c>
+      <c r="N70" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="O70" s="22" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="71" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="Q70" s="14"/>
+      <c r="R70" s="14"/>
+      <c r="S70" s="14"/>
+      <c r="T70" s="14"/>
+      <c r="U70" s="14"/>
+      <c r="V70" s="14"/>
+      <c r="W70" s="14"/>
+      <c r="X70" s="14"/>
+      <c r="Y70" s="14"/>
+      <c r="Z70" s="14"/>
+      <c r="AA70" s="14"/>
+      <c r="AB70" s="14"/>
+      <c r="AC70" s="14"/>
+      <c r="AD70" s="14"/>
+      <c r="AE70" s="14"/>
+      <c r="AF70" s="14"/>
+      <c r="AG70" s="14"/>
+      <c r="AH70" s="14"/>
+      <c r="AI70" s="14"/>
+      <c r="AJ70" s="14"/>
+      <c r="AK70" s="14"/>
+      <c r="AL70" s="14"/>
+      <c r="AM70" s="14"/>
+      <c r="AN70" s="14"/>
+      <c r="AO70" s="14"/>
+      <c r="AP70" s="14"/>
+      <c r="AQ70" s="14"/>
+      <c r="AR70" s="14"/>
+      <c r="AS70" s="14"/>
+      <c r="AT70" s="14"/>
+      <c r="AU70" s="14"/>
+      <c r="AV70" s="14"/>
+      <c r="AW70" s="14"/>
+      <c r="AX70" s="14"/>
+      <c r="AY70" s="14"/>
+      <c r="AZ70" s="14"/>
+      <c r="BA70" s="14"/>
+      <c r="BB70" s="14"/>
+      <c r="BC70" s="14"/>
+      <c r="BD70" s="14"/>
+      <c r="BE70" s="14"/>
+      <c r="BF70" s="14"/>
+      <c r="BG70" s="14"/>
+      <c r="BH70" s="14"/>
+      <c r="BI70" s="14"/>
+      <c r="BJ70" s="14"/>
+      <c r="BK70" s="14"/>
+      <c r="BL70" s="14"/>
+      <c r="BM70" s="14"/>
+    </row>
+    <row r="71" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>77</v>
+        <v>118</v>
       </c>
       <c r="B71" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C71" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D71" s="4" t="s">
+      <c r="C71" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F71" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G71" s="16">
+      <c r="G71" s="4">
         <v>403</v>
       </c>
       <c r="H71" s="35" t="s">
@@ -25679,94 +25759,45 @@
       <c r="I71" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J71" s="4" t="s">
+      <c r="J71" s="54" t="s">
         <v>40</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L71" s="5">
-        <v>1005</v>
+        <v>51</v>
+      </c>
+      <c r="L71" s="54">
+        <v>1015</v>
       </c>
       <c r="M71" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="N71" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="N71" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="O71" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q71" s="14"/>
-      <c r="R71" s="14"/>
-      <c r="S71" s="14"/>
-      <c r="T71" s="14"/>
-      <c r="U71" s="14"/>
-      <c r="V71" s="14"/>
-      <c r="W71" s="14"/>
-      <c r="X71" s="14"/>
-      <c r="Y71" s="14"/>
-      <c r="Z71" s="14"/>
-      <c r="AA71" s="14"/>
-      <c r="AB71" s="14"/>
-      <c r="AC71" s="14"/>
-      <c r="AD71" s="14"/>
-      <c r="AE71" s="14"/>
-      <c r="AF71" s="14"/>
-      <c r="AG71" s="14"/>
-      <c r="AH71" s="14"/>
-      <c r="AI71" s="14"/>
-      <c r="AJ71" s="14"/>
-      <c r="AK71" s="14"/>
-      <c r="AL71" s="14"/>
-      <c r="AM71" s="14"/>
-      <c r="AN71" s="14"/>
-      <c r="AO71" s="14"/>
-      <c r="AP71" s="14"/>
-      <c r="AQ71" s="14"/>
-      <c r="AR71" s="14"/>
-      <c r="AS71" s="14"/>
-      <c r="AT71" s="14"/>
-      <c r="AU71" s="14"/>
-      <c r="AV71" s="14"/>
-      <c r="AW71" s="14"/>
-      <c r="AX71" s="14"/>
-      <c r="AY71" s="14"/>
-      <c r="AZ71" s="14"/>
-      <c r="BA71" s="14"/>
-      <c r="BB71" s="14"/>
-      <c r="BC71" s="14"/>
-      <c r="BD71" s="14"/>
-      <c r="BE71" s="14"/>
-      <c r="BF71" s="14"/>
-      <c r="BG71" s="14"/>
-      <c r="BH71" s="14"/>
-      <c r="BI71" s="14"/>
-      <c r="BJ71" s="14"/>
-      <c r="BK71" s="14"/>
-      <c r="BL71" s="14"/>
-      <c r="BM71" s="14"/>
-    </row>
-    <row r="72" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="O71" s="55" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="72" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="B72" s="57" t="s">
         <v>155</v>
       </c>
-      <c r="C72" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D72" s="54" t="s">
+      <c r="C72" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E72" s="54" t="s">
+      <c r="E72" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F72" s="54" t="s">
+      <c r="F72" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G72" s="4">
+      <c r="G72" s="16">
         <v>403</v>
       </c>
       <c r="H72" s="35" t="s">
@@ -25775,34 +25806,34 @@
       <c r="I72" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J72" s="54" t="s">
+      <c r="J72" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K72" s="4" t="s">
+      <c r="K72" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="L72" s="54">
-        <v>1015</v>
+      <c r="L72" s="17">
+        <v>1006</v>
       </c>
       <c r="M72" s="22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N72" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="O72" s="55" t="s">
-        <v>36</v>
+        <v>147</v>
+      </c>
+      <c r="O72" s="22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="73" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B73" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>36</v>
@@ -25826,13 +25857,13 @@
         <v>40</v>
       </c>
       <c r="K73" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L73" s="17">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="M73" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N73" s="22" t="s">
         <v>147</v>
@@ -25843,13 +25874,13 @@
     </row>
     <row r="74" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B74" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>36</v>
@@ -25876,10 +25907,10 @@
         <v>47</v>
       </c>
       <c r="L74" s="17">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="M74" s="22" t="s">
-        <v>60</v>
+        <v>156</v>
       </c>
       <c r="N74" s="22" t="s">
         <v>147</v>
@@ -25890,15 +25921,15 @@
     </row>
     <row r="75" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B75" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D75" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E75" s="4" t="s">
@@ -25920,32 +25951,32 @@
         <v>40</v>
       </c>
       <c r="K75" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="L75" s="17">
-        <v>1008</v>
-      </c>
-      <c r="M75" s="22" t="s">
-        <v>156</v>
+        <v>41</v>
+      </c>
+      <c r="L75" s="16">
+        <v>1011</v>
+      </c>
+      <c r="M75" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="N75" s="22" t="s">
         <v>147</v>
       </c>
       <c r="O75" s="22" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="76" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="76" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B76" s="57" t="s">
         <v>155</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D76" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D76" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E76" s="4" t="s">
@@ -25955,7 +25986,7 @@
         <v>37</v>
       </c>
       <c r="G76" s="16">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H76" s="35" t="s">
         <v>38</v>
@@ -25963,90 +25994,112 @@
       <c r="I76" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J76" s="16" t="s">
+      <c r="J76" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K76" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="L76" s="16">
-        <v>1011</v>
-      </c>
-      <c r="M76" s="23" t="s">
-        <v>64</v>
+      <c r="K76" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L76" s="5">
+        <v>2506</v>
+      </c>
+      <c r="M76" s="22" t="s">
+        <v>158</v>
       </c>
       <c r="N76" s="22" t="s">
         <v>147</v>
       </c>
       <c r="O76" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
-        <v>71</v>
-      </c>
-      <c r="B77" s="57" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G77" s="16">
-        <v>404</v>
-      </c>
-      <c r="H77" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="I77" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K77" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L77" s="5">
-        <v>2506</v>
-      </c>
-      <c r="M77" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="N77" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="O77" s="22" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="78" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="95" t="s">
+    <row r="77" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="95" t="s">
         <v>160</v>
       </c>
-      <c r="B78" s="96"/>
-      <c r="C78" s="96"/>
-      <c r="D78" s="96"/>
-      <c r="E78" s="96"/>
-      <c r="F78" s="96"/>
-      <c r="G78" s="96"/>
-      <c r="H78" s="96"/>
-      <c r="I78" s="96"/>
-      <c r="J78" s="96"/>
-      <c r="K78" s="96"/>
-      <c r="L78" s="96"/>
-      <c r="M78" s="96"/>
-      <c r="N78" s="96"/>
-      <c r="O78" s="96"/>
+      <c r="B77" s="96"/>
+      <c r="C77" s="96"/>
+      <c r="D77" s="96"/>
+      <c r="E77" s="96"/>
+      <c r="F77" s="96"/>
+      <c r="G77" s="96"/>
+      <c r="H77" s="96"/>
+      <c r="I77" s="96"/>
+      <c r="J77" s="96"/>
+      <c r="K77" s="96"/>
+      <c r="L77" s="96"/>
+      <c r="M77" s="96"/>
+      <c r="N77" s="96"/>
+      <c r="O77" s="96"/>
+      <c r="P77" s="13"/>
+      <c r="Q77" s="13"/>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="13"/>
+      <c r="U77" s="13"/>
+      <c r="V77" s="13"/>
+      <c r="W77" s="13"/>
+      <c r="X77" s="13"/>
+      <c r="Y77" s="13"/>
+      <c r="Z77" s="13"/>
+      <c r="AA77" s="13"/>
+      <c r="AB77" s="13"/>
+      <c r="AC77" s="13"/>
+      <c r="AD77" s="13"/>
+      <c r="AE77" s="13"/>
+      <c r="AF77" s="13"/>
+      <c r="AG77" s="13"/>
+      <c r="AH77" s="13"/>
+      <c r="AI77" s="13"/>
+      <c r="AJ77" s="13"/>
+      <c r="AK77" s="13"/>
+      <c r="AL77" s="13"/>
+      <c r="AM77" s="13"/>
+      <c r="AN77" s="13"/>
+      <c r="AO77" s="13"/>
+      <c r="AP77" s="13"/>
+      <c r="AQ77" s="13"/>
+      <c r="AR77" s="13"/>
+      <c r="AS77" s="13"/>
+      <c r="AT77" s="13"/>
+      <c r="AU77" s="13"/>
+      <c r="AV77" s="13"/>
+      <c r="AW77" s="13"/>
+      <c r="AX77" s="13"/>
+      <c r="AY77" s="13"/>
+      <c r="AZ77" s="13"/>
+      <c r="BA77" s="13"/>
+      <c r="BB77" s="13"/>
+      <c r="BC77" s="13"/>
+      <c r="BD77" s="13"/>
+      <c r="BE77" s="13"/>
+      <c r="BF77" s="13"/>
+      <c r="BG77" s="13"/>
+      <c r="BH77" s="13"/>
+      <c r="BI77" s="13"/>
+      <c r="BJ77" s="13"/>
+      <c r="BK77" s="13"/>
+      <c r="BL77" s="13"/>
+      <c r="BM77" s="13"/>
+    </row>
+    <row r="78" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B78" s="98"/>
+      <c r="C78" s="98"/>
+      <c r="D78" s="98"/>
+      <c r="E78" s="98"/>
+      <c r="F78" s="98"/>
+      <c r="G78" s="98"/>
+      <c r="H78" s="98"/>
+      <c r="I78" s="98"/>
+      <c r="J78" s="98"/>
+      <c r="K78" s="98"/>
+      <c r="L78" s="98"/>
+      <c r="M78" s="98"/>
+      <c r="N78" s="98"/>
+      <c r="O78" s="98"/>
       <c r="P78" s="13"/>
       <c r="Q78" s="13"/>
       <c r="R78" s="13"/>
@@ -26098,24 +26151,52 @@
       <c r="BL78" s="13"/>
       <c r="BM78" s="13"/>
     </row>
-    <row r="79" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="B79" s="98"/>
-      <c r="C79" s="98"/>
-      <c r="D79" s="98"/>
-      <c r="E79" s="98"/>
-      <c r="F79" s="98"/>
-      <c r="G79" s="98"/>
-      <c r="H79" s="98"/>
-      <c r="I79" s="98"/>
-      <c r="J79" s="98"/>
-      <c r="K79" s="98"/>
-      <c r="L79" s="98"/>
-      <c r="M79" s="98"/>
-      <c r="N79" s="98"/>
-      <c r="O79" s="98"/>
+    <row r="79" spans="1:65" s="6" customFormat="1" ht="40.700000000000003" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="44">
+        <v>146</v>
+      </c>
+      <c r="B79" s="57" t="s">
+        <v>161</v>
+      </c>
+      <c r="C79" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="E79" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F79" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="G79" s="44">
+        <v>403</v>
+      </c>
+      <c r="H79" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="I79" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J79" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K79" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="L79" s="44">
+        <v>1016</v>
+      </c>
+      <c r="M79" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N79" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O79" s="45" t="s">
+        <v>36</v>
+      </c>
       <c r="P79" s="13"/>
       <c r="Q79" s="13"/>
       <c r="R79" s="13"/>
@@ -26167,50 +26248,50 @@
       <c r="BL79" s="13"/>
       <c r="BM79" s="13"/>
     </row>
-    <row r="80" spans="1:65" s="6" customFormat="1" ht="40.700000000000003" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="44">
-        <v>146</v>
+    <row r="80" spans="1:65" s="6" customFormat="1" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>72</v>
       </c>
       <c r="B80" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C80" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D80" s="44" t="s">
+      <c r="C80" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E80" s="44" t="s">
+      <c r="E80" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F80" s="44" t="s">
+      <c r="F80" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G80" s="44">
-        <v>403</v>
-      </c>
-      <c r="H80" s="44" t="s">
+      <c r="G80" s="16">
+        <v>401</v>
+      </c>
+      <c r="H80" s="35" t="s">
         <v>38</v>
       </c>
       <c r="I80" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J80" s="44" t="s">
+      <c r="J80" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K80" s="44" t="s">
+      <c r="K80" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L80" s="44">
-        <v>1016</v>
-      </c>
-      <c r="M80" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="N80" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="O80" s="45" t="s">
+      <c r="L80" s="4">
+        <v>1012</v>
+      </c>
+      <c r="M80" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N80" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O80" s="30" t="s">
         <v>36</v>
       </c>
       <c r="P80" s="13"/>
@@ -26264,15 +26345,15 @@
       <c r="BL80" s="13"/>
       <c r="BM80" s="13"/>
     </row>
-    <row r="81" spans="1:65" s="6" customFormat="1" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B81" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>36</v>
@@ -26299,15 +26380,15 @@
         <v>41</v>
       </c>
       <c r="L81" s="4">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="M81" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N81" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="O81" s="30" t="s">
+      <c r="O81" s="29" t="s">
         <v>36</v>
       </c>
       <c r="P81" s="13"/>
@@ -26361,15 +26442,15 @@
       <c r="BL81" s="13"/>
       <c r="BM81" s="13"/>
     </row>
-    <row r="82" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B82" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C82" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>36</v>
@@ -26381,7 +26462,7 @@
         <v>37</v>
       </c>
       <c r="G82" s="16">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="H82" s="35" t="s">
         <v>38</v>
@@ -26393,80 +26474,79 @@
         <v>40</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L82" s="4">
-        <v>1013</v>
-      </c>
-      <c r="M82" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="N82" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="O82" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="P82" s="13"/>
-      <c r="Q82" s="13"/>
-      <c r="R82" s="13"/>
-      <c r="S82" s="13"/>
-      <c r="T82" s="13"/>
-      <c r="U82" s="13"/>
-      <c r="V82" s="13"/>
-      <c r="W82" s="13"/>
-      <c r="X82" s="13"/>
-      <c r="Y82" s="13"/>
-      <c r="Z82" s="13"/>
-      <c r="AA82" s="13"/>
-      <c r="AB82" s="13"/>
-      <c r="AC82" s="13"/>
-      <c r="AD82" s="13"/>
-      <c r="AE82" s="13"/>
-      <c r="AF82" s="13"/>
-      <c r="AG82" s="13"/>
-      <c r="AH82" s="13"/>
-      <c r="AI82" s="13"/>
-      <c r="AJ82" s="13"/>
-      <c r="AK82" s="13"/>
-      <c r="AL82" s="13"/>
-      <c r="AM82" s="13"/>
-      <c r="AN82" s="13"/>
-      <c r="AO82" s="13"/>
-      <c r="AP82" s="13"/>
-      <c r="AQ82" s="13"/>
-      <c r="AR82" s="13"/>
-      <c r="AS82" s="13"/>
-      <c r="AT82" s="13"/>
-      <c r="AU82" s="13"/>
-      <c r="AV82" s="13"/>
-      <c r="AW82" s="13"/>
-      <c r="AX82" s="13"/>
-      <c r="AY82" s="13"/>
-      <c r="AZ82" s="13"/>
-      <c r="BA82" s="13"/>
-      <c r="BB82" s="13"/>
-      <c r="BC82" s="13"/>
-      <c r="BD82" s="13"/>
-      <c r="BE82" s="13"/>
-      <c r="BF82" s="13"/>
-      <c r="BG82" s="13"/>
-      <c r="BH82" s="13"/>
-      <c r="BI82" s="13"/>
-      <c r="BJ82" s="13"/>
-      <c r="BK82" s="13"/>
-      <c r="BL82" s="13"/>
-      <c r="BM82" s="13"/>
+        <v>47</v>
+      </c>
+      <c r="L82" s="5">
+        <v>1003</v>
+      </c>
+      <c r="M82" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="N82" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="O82" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q82" s="14"/>
+      <c r="R82" s="14"/>
+      <c r="S82" s="14"/>
+      <c r="T82" s="14"/>
+      <c r="U82" s="14"/>
+      <c r="V82" s="14"/>
+      <c r="W82" s="14"/>
+      <c r="X82" s="14"/>
+      <c r="Y82" s="14"/>
+      <c r="Z82" s="14"/>
+      <c r="AA82" s="14"/>
+      <c r="AB82" s="14"/>
+      <c r="AC82" s="14"/>
+      <c r="AD82" s="14"/>
+      <c r="AE82" s="14"/>
+      <c r="AF82" s="14"/>
+      <c r="AG82" s="14"/>
+      <c r="AH82" s="14"/>
+      <c r="AI82" s="14"/>
+      <c r="AJ82" s="14"/>
+      <c r="AK82" s="14"/>
+      <c r="AL82" s="14"/>
+      <c r="AM82" s="14"/>
+      <c r="AN82" s="14"/>
+      <c r="AO82" s="14"/>
+      <c r="AP82" s="14"/>
+      <c r="AQ82" s="14"/>
+      <c r="AR82" s="14"/>
+      <c r="AS82" s="14"/>
+      <c r="AT82" s="14"/>
+      <c r="AU82" s="14"/>
+      <c r="AV82" s="14"/>
+      <c r="AW82" s="14"/>
+      <c r="AX82" s="14"/>
+      <c r="AY82" s="14"/>
+      <c r="AZ82" s="14"/>
+      <c r="BA82" s="14"/>
+      <c r="BB82" s="14"/>
+      <c r="BC82" s="14"/>
+      <c r="BD82" s="14"/>
+      <c r="BE82" s="14"/>
+      <c r="BF82" s="14"/>
+      <c r="BG82" s="14"/>
+      <c r="BH82" s="14"/>
+      <c r="BI82" s="14"/>
+      <c r="BJ82" s="14"/>
+      <c r="BK82" s="14"/>
+      <c r="BL82" s="14"/>
+      <c r="BM82" s="14"/>
     </row>
     <row r="83" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B83" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C83" s="15" t="s">
-        <v>46</v>
+      <c r="C83" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>36</v>
@@ -26478,7 +26558,7 @@
         <v>37</v>
       </c>
       <c r="G83" s="16">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H83" s="35" t="s">
         <v>38</v>
@@ -26490,13 +26570,13 @@
         <v>40</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="L83" s="5">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="M83" s="22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="N83" s="22" t="s">
         <v>162</v>
@@ -26554,15 +26634,15 @@
       <c r="BL83" s="14"/>
       <c r="BM83" s="14"/>
     </row>
-    <row r="84" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B84" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>36</v>
@@ -26574,7 +26654,7 @@
         <v>37</v>
       </c>
       <c r="G84" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H84" s="35" t="s">
         <v>38</v>
@@ -26586,13 +26666,13 @@
         <v>40</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L84" s="5">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="M84" s="22" t="s">
-        <v>150</v>
+        <v>54</v>
       </c>
       <c r="N84" s="22" t="s">
         <v>162</v>
@@ -26650,26 +26730,26 @@
       <c r="BL84" s="14"/>
       <c r="BM84" s="14"/>
     </row>
-    <row r="85" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="B85" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C85" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D85" s="4" t="s">
+      <c r="C85" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D85" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F85" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="G85" s="16">
+      <c r="G85" s="4">
         <v>403</v>
       </c>
       <c r="H85" s="35" t="s">
@@ -26678,23 +26758,23 @@
       <c r="I85" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="J85" s="54" t="s">
         <v>40</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L85" s="5">
-        <v>1005</v>
+        <v>51</v>
+      </c>
+      <c r="L85" s="54">
+        <v>1015</v>
       </c>
       <c r="M85" s="22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N85" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="O85" s="22" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="O85" s="55" t="s">
+        <v>36</v>
       </c>
       <c r="Q85" s="14"/>
       <c r="R85" s="14"/>
@@ -26746,26 +26826,26 @@
       <c r="BL85" s="14"/>
       <c r="BM85" s="14"/>
     </row>
-    <row r="86" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="B86" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C86" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D86" s="54" t="s">
+      <c r="C86" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D86" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E86" s="54" t="s">
+      <c r="E86" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F86" s="54" t="s">
+      <c r="F86" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G86" s="4">
+      <c r="G86" s="16">
         <v>403</v>
       </c>
       <c r="H86" s="35" t="s">
@@ -26774,23 +26854,23 @@
       <c r="I86" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J86" s="54" t="s">
+      <c r="J86" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L86" s="54">
-        <v>1015</v>
+      <c r="L86" s="5">
+        <v>1006</v>
       </c>
       <c r="M86" s="22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="N86" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="O86" s="55" t="s">
-        <v>36</v>
+        <v>162</v>
+      </c>
+      <c r="O86" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="Q86" s="14"/>
       <c r="R86" s="14"/>
@@ -26844,13 +26924,13 @@
     </row>
     <row r="87" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B87" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>36</v>
@@ -26874,13 +26954,13 @@
         <v>40</v>
       </c>
       <c r="K87" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L87" s="5">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="M87" s="22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="N87" s="22" t="s">
         <v>162</v>
@@ -26938,15 +27018,15 @@
       <c r="BL87" s="14"/>
       <c r="BM87" s="14"/>
     </row>
-    <row r="88" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B88" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>36</v>
@@ -26973,10 +27053,10 @@
         <v>47</v>
       </c>
       <c r="L88" s="5">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="M88" s="22" t="s">
-        <v>60</v>
+        <v>163</v>
       </c>
       <c r="N88" s="22" t="s">
         <v>162</v>
@@ -27036,13 +27116,13 @@
     </row>
     <row r="89" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B89" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>61</v>
+        <v>164</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>36</v>
@@ -27066,19 +27146,19 @@
         <v>40</v>
       </c>
       <c r="K89" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L89" s="5">
-        <v>1008</v>
+        <v>1011</v>
       </c>
       <c r="M89" s="22" t="s">
-        <v>163</v>
+        <v>64</v>
       </c>
       <c r="N89" s="22" t="s">
         <v>162</v>
       </c>
       <c r="O89" s="22" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="Q89" s="14"/>
       <c r="R89" s="14"/>
@@ -27130,15 +27210,15 @@
       <c r="BL89" s="14"/>
       <c r="BM89" s="14"/>
     </row>
-    <row r="90" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
-        <v>81</v>
+    <row r="90" spans="1:65" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="18">
+        <v>169</v>
       </c>
       <c r="B90" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C90" s="3" t="s">
-        <v>164</v>
+      <c r="C90" s="51" t="s">
+        <v>165</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>36</v>
@@ -27150,7 +27230,7 @@
         <v>37</v>
       </c>
       <c r="G90" s="16">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="H90" s="35" t="s">
         <v>38</v>
@@ -27162,90 +27242,91 @@
         <v>40</v>
       </c>
       <c r="K90" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L90" s="5">
-        <v>1011</v>
-      </c>
-      <c r="M90" s="22" t="s">
-        <v>64</v>
+        <v>47</v>
+      </c>
+      <c r="L90" s="18">
+        <v>3101</v>
+      </c>
+      <c r="M90" s="40" t="s">
+        <v>166</v>
       </c>
       <c r="N90" s="22" t="s">
         <v>162</v>
       </c>
       <c r="O90" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q90" s="14"/>
-      <c r="R90" s="14"/>
-      <c r="S90" s="14"/>
-      <c r="T90" s="14"/>
-      <c r="U90" s="14"/>
-      <c r="V90" s="14"/>
-      <c r="W90" s="14"/>
-      <c r="X90" s="14"/>
-      <c r="Y90" s="14"/>
-      <c r="Z90" s="14"/>
-      <c r="AA90" s="14"/>
-      <c r="AB90" s="14"/>
-      <c r="AC90" s="14"/>
-      <c r="AD90" s="14"/>
-      <c r="AE90" s="14"/>
-      <c r="AF90" s="14"/>
-      <c r="AG90" s="14"/>
-      <c r="AH90" s="14"/>
-      <c r="AI90" s="14"/>
-      <c r="AJ90" s="14"/>
-      <c r="AK90" s="14"/>
-      <c r="AL90" s="14"/>
-      <c r="AM90" s="14"/>
-      <c r="AN90" s="14"/>
-      <c r="AO90" s="14"/>
-      <c r="AP90" s="14"/>
-      <c r="AQ90" s="14"/>
-      <c r="AR90" s="14"/>
-      <c r="AS90" s="14"/>
-      <c r="AT90" s="14"/>
-      <c r="AU90" s="14"/>
-      <c r="AV90" s="14"/>
-      <c r="AW90" s="14"/>
-      <c r="AX90" s="14"/>
-      <c r="AY90" s="14"/>
-      <c r="AZ90" s="14"/>
-      <c r="BA90" s="14"/>
-      <c r="BB90" s="14"/>
-      <c r="BC90" s="14"/>
-      <c r="BD90" s="14"/>
-      <c r="BE90" s="14"/>
-      <c r="BF90" s="14"/>
-      <c r="BG90" s="14"/>
-      <c r="BH90" s="14"/>
-      <c r="BI90" s="14"/>
-      <c r="BJ90" s="14"/>
-      <c r="BK90" s="14"/>
-      <c r="BL90" s="14"/>
-      <c r="BM90" s="14"/>
-    </row>
-    <row r="91" spans="1:65" s="6" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="18">
-        <v>169</v>
+        <v>167</v>
+      </c>
+      <c r="P90" s="13"/>
+      <c r="Q90" s="13"/>
+      <c r="R90" s="13"/>
+      <c r="S90" s="13"/>
+      <c r="T90" s="13"/>
+      <c r="U90" s="13"/>
+      <c r="V90" s="13"/>
+      <c r="W90" s="13"/>
+      <c r="X90" s="13"/>
+      <c r="Y90" s="13"/>
+      <c r="Z90" s="13"/>
+      <c r="AA90" s="13"/>
+      <c r="AB90" s="13"/>
+      <c r="AC90" s="13"/>
+      <c r="AD90" s="13"/>
+      <c r="AE90" s="13"/>
+      <c r="AF90" s="13"/>
+      <c r="AG90" s="13"/>
+      <c r="AH90" s="13"/>
+      <c r="AI90" s="13"/>
+      <c r="AJ90" s="13"/>
+      <c r="AK90" s="13"/>
+      <c r="AL90" s="13"/>
+      <c r="AM90" s="13"/>
+      <c r="AN90" s="13"/>
+      <c r="AO90" s="13"/>
+      <c r="AP90" s="13"/>
+      <c r="AQ90" s="13"/>
+      <c r="AR90" s="13"/>
+      <c r="AS90" s="13"/>
+      <c r="AT90" s="13"/>
+      <c r="AU90" s="13"/>
+      <c r="AV90" s="13"/>
+      <c r="AW90" s="13"/>
+      <c r="AX90" s="13"/>
+      <c r="AY90" s="13"/>
+      <c r="AZ90" s="13"/>
+      <c r="BA90" s="13"/>
+      <c r="BB90" s="13"/>
+      <c r="BC90" s="13"/>
+      <c r="BD90" s="13"/>
+      <c r="BE90" s="13"/>
+      <c r="BF90" s="13"/>
+      <c r="BG90" s="13"/>
+      <c r="BH90" s="13"/>
+      <c r="BI90" s="13"/>
+      <c r="BJ90" s="13"/>
+      <c r="BK90" s="13"/>
+      <c r="BL90" s="13"/>
+      <c r="BM90" s="13"/>
+    </row>
+    <row r="91" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="35">
+        <v>156</v>
       </c>
       <c r="B91" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C91" s="51" t="s">
-        <v>165</v>
-      </c>
-      <c r="D91" s="4" t="s">
+      <c r="C91" s="47" t="s">
+        <v>168</v>
+      </c>
+      <c r="D91" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E91" s="4" t="s">
+      <c r="E91" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="F91" s="4" t="s">
+      <c r="F91" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G91" s="16">
+      <c r="G91" s="35">
         <v>400</v>
       </c>
       <c r="H91" s="35" t="s">
@@ -27254,23 +27335,23 @@
       <c r="I91" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="J91" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="K91" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L91" s="18">
-        <v>3101</v>
-      </c>
-      <c r="M91" s="40" t="s">
-        <v>166</v>
+      <c r="K91" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="L91" s="35">
+        <v>3014</v>
+      </c>
+      <c r="M91" s="47" t="s">
+        <v>169</v>
       </c>
       <c r="N91" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="O91" s="22" t="s">
-        <v>167</v>
+      <c r="O91" s="58" t="s">
+        <v>170</v>
       </c>
       <c r="P91" s="13"/>
       <c r="Q91" s="13"/>
@@ -27323,115 +27404,65 @@
       <c r="BL91" s="13"/>
       <c r="BM91" s="13"/>
     </row>
-    <row r="92" spans="1:65" s="6" customFormat="1" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="35">
-        <v>156</v>
+    <row r="92" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>168</v>
       </c>
       <c r="B92" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="C92" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="D92" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="E92" s="35" t="s">
+      <c r="C92" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D92" s="4">
+        <v>9</v>
+      </c>
+      <c r="E92" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="F92" s="35" t="s">
+      <c r="F92" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G92" s="35">
-        <v>400</v>
-      </c>
-      <c r="H92" s="35" t="s">
-        <v>38</v>
+      <c r="G92" s="16">
+        <v>200</v>
+      </c>
+      <c r="H92" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="I92" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J92" s="35" t="s">
+      <c r="J92" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K92" s="35" t="s">
+      <c r="K92" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L92" s="35">
-        <v>3014</v>
-      </c>
-      <c r="M92" s="47" t="s">
-        <v>169</v>
+      <c r="L92" s="4">
+        <v>1010</v>
+      </c>
+      <c r="M92" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="N92" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="O92" s="58" t="s">
-        <v>170</v>
-      </c>
-      <c r="P92" s="13"/>
-      <c r="Q92" s="13"/>
-      <c r="R92" s="13"/>
-      <c r="S92" s="13"/>
-      <c r="T92" s="13"/>
-      <c r="U92" s="13"/>
-      <c r="V92" s="13"/>
-      <c r="W92" s="13"/>
-      <c r="X92" s="13"/>
-      <c r="Y92" s="13"/>
-      <c r="Z92" s="13"/>
-      <c r="AA92" s="13"/>
-      <c r="AB92" s="13"/>
-      <c r="AC92" s="13"/>
-      <c r="AD92" s="13"/>
-      <c r="AE92" s="13"/>
-      <c r="AF92" s="13"/>
-      <c r="AG92" s="13"/>
-      <c r="AH92" s="13"/>
-      <c r="AI92" s="13"/>
-      <c r="AJ92" s="13"/>
-      <c r="AK92" s="13"/>
-      <c r="AL92" s="13"/>
-      <c r="AM92" s="13"/>
-      <c r="AN92" s="13"/>
-      <c r="AO92" s="13"/>
-      <c r="AP92" s="13"/>
-      <c r="AQ92" s="13"/>
-      <c r="AR92" s="13"/>
-      <c r="AS92" s="13"/>
-      <c r="AT92" s="13"/>
-      <c r="AU92" s="13"/>
-      <c r="AV92" s="13"/>
-      <c r="AW92" s="13"/>
-      <c r="AX92" s="13"/>
-      <c r="AY92" s="13"/>
-      <c r="AZ92" s="13"/>
-      <c r="BA92" s="13"/>
-      <c r="BB92" s="13"/>
-      <c r="BC92" s="13"/>
-      <c r="BD92" s="13"/>
-      <c r="BE92" s="13"/>
-      <c r="BF92" s="13"/>
-      <c r="BG92" s="13"/>
-      <c r="BH92" s="13"/>
-      <c r="BI92" s="13"/>
-      <c r="BJ92" s="13"/>
-      <c r="BK92" s="13"/>
-      <c r="BL92" s="13"/>
-      <c r="BM92" s="13"/>
+      <c r="O92" s="22" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="93" spans="1:65" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B93" s="57" t="s">
         <v>161</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D93" s="4">
-        <v>9</v>
+        <v>188</v>
+      </c>
+      <c r="D93" s="35" t="s">
+        <v>36</v>
       </c>
       <c r="E93" s="16" t="s">
         <v>37</v>
@@ -27455,16 +27486,16 @@
         <v>51</v>
       </c>
       <c r="L93" s="4">
-        <v>1010</v>
+        <v>3015</v>
       </c>
       <c r="M93" s="22" t="s">
-        <v>99</v>
+        <v>187</v>
       </c>
       <c r="N93" s="22" t="s">
         <v>162</v>
       </c>
       <c r="O93" s="22" t="s">
-        <v>100</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -32175,27 +32206,27 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A63:O63"/>
+    <mergeCell ref="A62:O62"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A19:O19"/>
+    <mergeCell ref="A47:O47"/>
     <mergeCell ref="A48:O48"/>
-    <mergeCell ref="A49:O49"/>
     <mergeCell ref="A94:O94"/>
     <mergeCell ref="A95:O95"/>
+    <mergeCell ref="A77:O77"/>
+    <mergeCell ref="A63:O63"/>
     <mergeCell ref="A78:O78"/>
-    <mergeCell ref="A64:O64"/>
-    <mergeCell ref="A79:O79"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L58:L62 L11:L15 L73:L77 L23:L24 L31:L32 L17:L18 L7:L9 L69:L71 L54:L56 L26:L29 L87:L90 L93 L83:L85 L99:L101 L103:L108" xr:uid="{8072A8F1-1A15-4450-88CE-A1709A757457}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L57:L61 L11:L15 L72:L76 L23:L24 L31:L32 L17:L18 L7:L9 L68:L70 L53:L55 L26:L29 L86:L89 L103:L108 L82:L84 L99:L101 L92" xr:uid="{8072A8F1-1A15-4450-88CE-A1709A757457}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K58:K62 K73:K77 K69:K71 K7:K9 K54:K56 K11:K18 K87:K93 K83:K85 K103:K109 K99:K101 K23:K45" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K57:K61 K72:K76 K68:K70 K7:K9 K53:K55 K11:K18 K23:K45 K82:K84 K103:K109 K99:K101 K86:K93" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
       <formula1>"Field,Cross Field,Cross Form"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J58:J62 J73:J77 J69:J71 J7:J9 J54:J56 J11:J18 J87:J93 J83:J85 J103:J109 J99:J101 J23:J45" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J57:J61 J72:J76 J68:J70 J7:J9 J53:J55 J11:J18 J23:J45 J82:J84 J103:J109 J99:J101 J86:J93" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
       <formula1>"Error,Warning"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update to ERR Validation Rules
</commit_message>
<xml_diff>
--- a/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
+++ b/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC6B4A-309D-4B0B-A7AF-D6D04101D463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81011158-3B54-438F-8BB7-A683ABDD2BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="0" windowWidth="18420" windowHeight="14520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="202">
   <si>
     <t xml:space="preserve">Latest Version History </t>
   </si>
@@ -411,18 +411,6 @@
     <t>Number of days exceeds -365 or Number of days exceeds -366 in a leap year</t>
   </si>
   <si>
-    <t>Small Benefit value can not exceed 1000 (value  may change in future)</t>
-  </si>
-  <si>
-    <t>Value of Benefit can not exceed €1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small Benefit can not be entered more than twice for PPSN in one tax year </t>
-  </si>
-  <si>
-    <t>Exemption can not exceed 2 per employee per tax year</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -630,12 +618,51 @@
   <si>
     <t>Removed 173</t>
   </si>
+  <si>
+    <t>Small Benefit value can not exceed 1500 (value  may change in future)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small Benefit can not be entered more than five times for PPSN in one tax year </t>
+  </si>
+  <si>
+    <t>Changed max amount from 1000 to 1500</t>
+  </si>
+  <si>
+    <t>Changed max small benefits amount from 2 to 5</t>
+  </si>
+  <si>
+    <t>Value of benefit exceeds allowable amount</t>
+  </si>
+  <si>
+    <t>Exemption exceeds maximum number  allowable per year</t>
+  </si>
+  <si>
+    <t>Appendix A</t>
+  </si>
+  <si>
+    <t>Small Benefit value can not exceed 1000 (value  may change in future)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small Benefit can not be entered more than twice for PPSN in one tax year </t>
+  </si>
+  <si>
+    <t>See Appendix A below for allowable amounts for specific years</t>
+  </si>
+  <si>
+    <t>See Appendix A below for allowable number of submissions for specific years</t>
+  </si>
+  <si>
+    <t>Small Benefit Exemption rules applicable up to 31/12/2024</t>
+  </si>
+  <si>
+    <t>Small Benefit Exmption rules applicable from 01/01/2025 Onwards</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -762,8 +789,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -813,6 +855,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -974,12 +1022,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1232,6 +1281,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1252,6 +1307,18 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1280,12 +1347,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -21660,9 +21734,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -21700,9 +21774,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -21735,26 +21809,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -21787,26 +21844,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -21983,7 +22023,7 @@
   <dimension ref="B8:E68"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21998,18 +22038,18 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="88" t="s">
+      <c r="B8" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="90"/>
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
@@ -22050,7 +22090,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="89">
+      <c r="B14" s="91">
         <v>0.12</v>
       </c>
       <c r="C14" s="71">
@@ -22059,59 +22099,59 @@
       <c r="D14" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="92">
+      <c r="E14" s="94">
         <v>45218</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="90"/>
+      <c r="B15" s="92"/>
       <c r="C15" s="34" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="93"/>
+      <c r="E15" s="95"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="90"/>
+      <c r="B16" s="92"/>
       <c r="C16" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="93"/>
+      <c r="E16" s="95"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="90"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="71" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="93"/>
+      <c r="E17" s="95"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="91"/>
+      <c r="B18" s="93"/>
       <c r="C18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="94"/>
+      <c r="E18" s="96"/>
     </row>
     <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="59">
         <v>0.13</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E19" s="70">
         <v>45272</v>
@@ -22122,12 +22162,12 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="E20" s="104">
+        <v>187</v>
+      </c>
+      <c r="E20" s="88">
         <v>45371</v>
       </c>
     </row>
@@ -22139,23 +22179,37 @@
         <v>173</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E21" s="70">
         <v>45373</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="21"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="63"/>
+      <c r="B22" s="21">
+        <v>0.16</v>
+      </c>
+      <c r="C22" s="34">
+        <v>38</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="70">
+        <v>45582</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="21"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="63"/>
+      <c r="C23" s="34">
+        <v>39</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="E23" s="70">
+        <v>45582</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="21"/>
@@ -22444,10 +22498,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BM342"/>
+  <dimension ref="A1:BM345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -22516,43 +22570,43 @@
       <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="100"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="106"/>
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="99"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="105"/>
       <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -23314,23 +23368,23 @@
       <c r="P18" s="24"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="97" t="s">
+      <c r="A19" s="103" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="98"/>
-      <c r="C19" s="98"/>
-      <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="98"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="98"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="98"/>
-      <c r="L19" s="98"/>
-      <c r="M19" s="98"/>
-      <c r="N19" s="98"/>
-      <c r="O19" s="99"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
+      <c r="J19" s="104"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="104"/>
+      <c r="M19" s="104"/>
+      <c r="N19" s="104"/>
+      <c r="O19" s="105"/>
       <c r="P19" s="13"/>
     </row>
     <row r="20" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -24189,8 +24243,8 @@
       <c r="B38" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="19" t="s">
-        <v>128</v>
+      <c r="C38" s="89" t="s">
+        <v>198</v>
       </c>
       <c r="D38" s="4">
         <v>17</v>
@@ -24216,11 +24270,11 @@
       <c r="K38" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L38" s="5">
+      <c r="L38" s="110">
         <v>2603</v>
       </c>
-      <c r="M38" s="43" t="s">
-        <v>129</v>
+      <c r="M38" s="111" t="s">
+        <v>193</v>
       </c>
       <c r="N38" s="22" t="s">
         <v>77</v>
@@ -24236,8 +24290,8 @@
       <c r="B39" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="19" t="s">
-        <v>130</v>
+      <c r="C39" s="89" t="s">
+        <v>199</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>36</v>
@@ -24263,17 +24317,17 @@
       <c r="K39" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L39" s="5">
+      <c r="L39" s="110">
         <v>2604</v>
       </c>
-      <c r="M39" s="50" t="s">
-        <v>131</v>
+      <c r="M39" s="112" t="s">
+        <v>194</v>
       </c>
       <c r="N39" s="22" t="s">
         <v>77</v>
       </c>
       <c r="O39" s="22" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -24284,7 +24338,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>36</v>
@@ -24331,7 +24385,7 @@
         <v>34</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>36</v>
@@ -24361,7 +24415,7 @@
         <v>2606</v>
       </c>
       <c r="M41" s="43" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="N41" s="22" t="s">
         <v>77</v>
@@ -24378,7 +24432,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>36</v>
@@ -24417,7 +24471,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>170</v>
       </c>
@@ -24425,7 +24479,7 @@
         <v>34</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D43" s="4">
         <v>19</v>
@@ -24455,7 +24509,7 @@
         <v>2609</v>
       </c>
       <c r="M43" s="50" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="N43" s="22" t="s">
         <v>77</v>
@@ -24472,7 +24526,7 @@
         <v>34</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>36</v>
@@ -24502,7 +24556,7 @@
         <v>2610</v>
       </c>
       <c r="M44" s="50" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="N44" s="22" t="s">
         <v>77</v>
@@ -24519,7 +24573,7 @@
         <v>34</v>
       </c>
       <c r="C45" s="77" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D45" s="75" t="s">
         <v>36</v>
@@ -24549,7 +24603,7 @@
         <v>2611</v>
       </c>
       <c r="M45" s="80" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N45" s="81" t="s">
         <v>77</v>
@@ -24566,7 +24620,7 @@
         <v>34</v>
       </c>
       <c r="C46" s="84" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D46" s="82" t="s">
         <v>36</v>
@@ -24596,53 +24650,53 @@
         <v>2614</v>
       </c>
       <c r="M46" s="87" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="N46" s="83" t="s">
         <v>77</v>
       </c>
       <c r="O46" s="83" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="101" t="s">
-        <v>143</v>
-      </c>
-      <c r="B47" s="102"/>
-      <c r="C47" s="102"/>
-      <c r="D47" s="102"/>
-      <c r="E47" s="102"/>
-      <c r="F47" s="102"/>
-      <c r="G47" s="102"/>
-      <c r="H47" s="102"/>
-      <c r="I47" s="102"/>
-      <c r="J47" s="102"/>
-      <c r="K47" s="102"/>
-      <c r="L47" s="102"/>
-      <c r="M47" s="102"/>
-      <c r="N47" s="102"/>
-      <c r="O47" s="103"/>
+      <c r="A47" s="107" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="108"/>
+      <c r="C47" s="108"/>
+      <c r="D47" s="108"/>
+      <c r="E47" s="108"/>
+      <c r="F47" s="108"/>
+      <c r="G47" s="108"/>
+      <c r="H47" s="108"/>
+      <c r="I47" s="108"/>
+      <c r="J47" s="108"/>
+      <c r="K47" s="108"/>
+      <c r="L47" s="108"/>
+      <c r="M47" s="108"/>
+      <c r="N47" s="108"/>
+      <c r="O47" s="109"/>
       <c r="P47" s="13"/>
     </row>
     <row r="48" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="97" t="s">
+      <c r="A48" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="98"/>
-      <c r="C48" s="98"/>
-      <c r="D48" s="98"/>
-      <c r="E48" s="98"/>
-      <c r="F48" s="98"/>
-      <c r="G48" s="98"/>
-      <c r="H48" s="98"/>
-      <c r="I48" s="98"/>
-      <c r="J48" s="98"/>
-      <c r="K48" s="98"/>
-      <c r="L48" s="98"/>
-      <c r="M48" s="98"/>
-      <c r="N48" s="98"/>
-      <c r="O48" s="99"/>
+      <c r="B48" s="104"/>
+      <c r="C48" s="104"/>
+      <c r="D48" s="104"/>
+      <c r="E48" s="104"/>
+      <c r="F48" s="104"/>
+      <c r="G48" s="104"/>
+      <c r="H48" s="104"/>
+      <c r="I48" s="104"/>
+      <c r="J48" s="104"/>
+      <c r="K48" s="104"/>
+      <c r="L48" s="104"/>
+      <c r="M48" s="104"/>
+      <c r="N48" s="104"/>
+      <c r="O48" s="105"/>
       <c r="P48" s="13"/>
     </row>
     <row r="49" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -24650,10 +24704,10 @@
         <v>148</v>
       </c>
       <c r="B49" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C49" s="45" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D49" s="44" t="s">
         <v>36</v>
@@ -24683,10 +24737,10 @@
         <v>1111</v>
       </c>
       <c r="M49" s="45" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N49" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O49" s="22" t="s">
         <v>58</v>
@@ -24698,7 +24752,7 @@
         <v>146</v>
       </c>
       <c r="B50" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C50" s="45" t="s">
         <v>35</v>
@@ -24746,7 +24800,7 @@
         <v>52</v>
       </c>
       <c r="B51" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C51" s="23" t="s">
         <v>43</v>
@@ -24794,7 +24848,7 @@
         <v>53</v>
       </c>
       <c r="B52" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>45</v>
@@ -24842,7 +24896,7 @@
         <v>55</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>46</v>
@@ -24875,10 +24929,10 @@
         <v>1003</v>
       </c>
       <c r="M53" s="23" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N53" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O53" s="22" t="s">
         <v>49</v>
@@ -24889,10 +24943,10 @@
         <v>56</v>
       </c>
       <c r="B54" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>36</v>
@@ -24922,10 +24976,10 @@
         <v>1004</v>
       </c>
       <c r="M54" s="23" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N54" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O54" s="22" t="s">
         <v>49</v>
@@ -24936,7 +24990,7 @@
         <v>77</v>
       </c>
       <c r="B55" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>53</v>
@@ -25032,7 +25086,7 @@
         <v>117</v>
       </c>
       <c r="B56" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C56" s="22" t="s">
         <v>55</v>
@@ -25079,7 +25133,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>56</v>
@@ -25115,7 +25169,7 @@
         <v>57</v>
       </c>
       <c r="N57" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O57" s="22" t="s">
         <v>58</v>
@@ -25126,7 +25180,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>59</v>
@@ -25162,7 +25216,7 @@
         <v>60</v>
       </c>
       <c r="N58" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O58" s="22" t="s">
         <v>58</v>
@@ -25173,10 +25227,10 @@
         <v>59</v>
       </c>
       <c r="B59" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>36</v>
@@ -25209,7 +25263,7 @@
         <v>62</v>
       </c>
       <c r="N59" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O59" s="22" t="s">
         <v>58</v>
@@ -25220,7 +25274,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>63</v>
@@ -25256,7 +25310,7 @@
         <v>64</v>
       </c>
       <c r="N60" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O60" s="22" t="s">
         <v>36</v>
@@ -25267,10 +25321,10 @@
         <v>61</v>
       </c>
       <c r="B61" s="57" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>36</v>
@@ -25300,7 +25354,7 @@
         <v>2501</v>
       </c>
       <c r="M61" s="22" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="N61" s="22" t="s">
         <v>67</v>
@@ -25310,43 +25364,43 @@
       </c>
     </row>
     <row r="62" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="95" t="s">
-        <v>154</v>
-      </c>
-      <c r="B62" s="96"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="96"/>
-      <c r="E62" s="96"/>
-      <c r="F62" s="96"/>
-      <c r="G62" s="96"/>
-      <c r="H62" s="96"/>
-      <c r="I62" s="96"/>
-      <c r="J62" s="96"/>
-      <c r="K62" s="96"/>
-      <c r="L62" s="96"/>
-      <c r="M62" s="96"/>
-      <c r="N62" s="96"/>
-      <c r="O62" s="100"/>
+      <c r="A62" s="101" t="s">
+        <v>150</v>
+      </c>
+      <c r="B62" s="102"/>
+      <c r="C62" s="102"/>
+      <c r="D62" s="102"/>
+      <c r="E62" s="102"/>
+      <c r="F62" s="102"/>
+      <c r="G62" s="102"/>
+      <c r="H62" s="102"/>
+      <c r="I62" s="102"/>
+      <c r="J62" s="102"/>
+      <c r="K62" s="102"/>
+      <c r="L62" s="102"/>
+      <c r="M62" s="102"/>
+      <c r="N62" s="102"/>
+      <c r="O62" s="106"/>
       <c r="P62" s="13"/>
     </row>
     <row r="63" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="97" t="s">
+      <c r="A63" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B63" s="98"/>
-      <c r="C63" s="98"/>
-      <c r="D63" s="98"/>
-      <c r="E63" s="98"/>
-      <c r="F63" s="98"/>
-      <c r="G63" s="98"/>
-      <c r="H63" s="98"/>
-      <c r="I63" s="98"/>
-      <c r="J63" s="98"/>
-      <c r="K63" s="98"/>
-      <c r="L63" s="98"/>
-      <c r="M63" s="98"/>
-      <c r="N63" s="98"/>
-      <c r="O63" s="99"/>
+      <c r="B63" s="104"/>
+      <c r="C63" s="104"/>
+      <c r="D63" s="104"/>
+      <c r="E63" s="104"/>
+      <c r="F63" s="104"/>
+      <c r="G63" s="104"/>
+      <c r="H63" s="104"/>
+      <c r="I63" s="104"/>
+      <c r="J63" s="104"/>
+      <c r="K63" s="104"/>
+      <c r="L63" s="104"/>
+      <c r="M63" s="104"/>
+      <c r="N63" s="104"/>
+      <c r="O63" s="105"/>
       <c r="P63" s="13"/>
     </row>
     <row r="64" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -25354,10 +25408,10 @@
         <v>148</v>
       </c>
       <c r="B64" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D64" s="44" t="s">
         <v>36</v>
@@ -25387,10 +25441,10 @@
         <v>1111</v>
       </c>
       <c r="M64" s="45" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N64" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O64" s="22" t="s">
         <v>58</v>
@@ -25402,7 +25456,7 @@
         <v>146</v>
       </c>
       <c r="B65" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C65" s="45" t="s">
         <v>35</v>
@@ -25450,7 +25504,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>43</v>
@@ -25498,7 +25552,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>45</v>
@@ -25546,7 +25600,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>46</v>
@@ -25582,7 +25636,7 @@
         <v>48</v>
       </c>
       <c r="N68" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O68" s="4" t="s">
         <v>49</v>
@@ -25593,10 +25647,10 @@
         <v>66</v>
       </c>
       <c r="B69" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>36</v>
@@ -25629,7 +25683,7 @@
         <v>52</v>
       </c>
       <c r="N69" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O69" s="22" t="s">
         <v>49</v>
@@ -25640,7 +25694,7 @@
         <v>77</v>
       </c>
       <c r="B70" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>53</v>
@@ -25736,7 +25790,7 @@
         <v>118</v>
       </c>
       <c r="B71" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>55</v>
@@ -25783,7 +25837,7 @@
         <v>67</v>
       </c>
       <c r="B72" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C72" s="15" t="s">
         <v>56</v>
@@ -25819,7 +25873,7 @@
         <v>57</v>
       </c>
       <c r="N72" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O72" s="22" t="s">
         <v>58</v>
@@ -25830,7 +25884,7 @@
         <v>68</v>
       </c>
       <c r="B73" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>59</v>
@@ -25866,7 +25920,7 @@
         <v>60</v>
       </c>
       <c r="N73" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O73" s="22" t="s">
         <v>58</v>
@@ -25877,7 +25931,7 @@
         <v>69</v>
       </c>
       <c r="B74" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>61</v>
@@ -25910,10 +25964,10 @@
         <v>1008</v>
       </c>
       <c r="M74" s="22" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="N74" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O74" s="22" t="s">
         <v>58</v>
@@ -25924,7 +25978,7 @@
         <v>70</v>
       </c>
       <c r="B75" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>63</v>
@@ -25960,7 +26014,7 @@
         <v>64</v>
       </c>
       <c r="N75" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O75" s="22" t="s">
         <v>36</v>
@@ -25971,10 +26025,10 @@
         <v>71</v>
       </c>
       <c r="B76" s="57" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>36</v>
@@ -26004,33 +26058,33 @@
         <v>2506</v>
       </c>
       <c r="M76" s="22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="N76" s="22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O76" s="22" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="95" t="s">
-        <v>160</v>
-      </c>
-      <c r="B77" s="96"/>
-      <c r="C77" s="96"/>
-      <c r="D77" s="96"/>
-      <c r="E77" s="96"/>
-      <c r="F77" s="96"/>
-      <c r="G77" s="96"/>
-      <c r="H77" s="96"/>
-      <c r="I77" s="96"/>
-      <c r="J77" s="96"/>
-      <c r="K77" s="96"/>
-      <c r="L77" s="96"/>
-      <c r="M77" s="96"/>
-      <c r="N77" s="96"/>
-      <c r="O77" s="96"/>
+      <c r="A77" s="101" t="s">
+        <v>156</v>
+      </c>
+      <c r="B77" s="102"/>
+      <c r="C77" s="102"/>
+      <c r="D77" s="102"/>
+      <c r="E77" s="102"/>
+      <c r="F77" s="102"/>
+      <c r="G77" s="102"/>
+      <c r="H77" s="102"/>
+      <c r="I77" s="102"/>
+      <c r="J77" s="102"/>
+      <c r="K77" s="102"/>
+      <c r="L77" s="102"/>
+      <c r="M77" s="102"/>
+      <c r="N77" s="102"/>
+      <c r="O77" s="102"/>
       <c r="P77" s="13"/>
       <c r="Q77" s="13"/>
       <c r="R77" s="13"/>
@@ -26083,23 +26137,23 @@
       <c r="BM77" s="13"/>
     </row>
     <row r="78" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="97" t="s">
+      <c r="A78" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="98"/>
-      <c r="C78" s="98"/>
-      <c r="D78" s="98"/>
-      <c r="E78" s="98"/>
-      <c r="F78" s="98"/>
-      <c r="G78" s="98"/>
-      <c r="H78" s="98"/>
-      <c r="I78" s="98"/>
-      <c r="J78" s="98"/>
-      <c r="K78" s="98"/>
-      <c r="L78" s="98"/>
-      <c r="M78" s="98"/>
-      <c r="N78" s="98"/>
-      <c r="O78" s="98"/>
+      <c r="B78" s="104"/>
+      <c r="C78" s="104"/>
+      <c r="D78" s="104"/>
+      <c r="E78" s="104"/>
+      <c r="F78" s="104"/>
+      <c r="G78" s="104"/>
+      <c r="H78" s="104"/>
+      <c r="I78" s="104"/>
+      <c r="J78" s="104"/>
+      <c r="K78" s="104"/>
+      <c r="L78" s="104"/>
+      <c r="M78" s="104"/>
+      <c r="N78" s="104"/>
+      <c r="O78" s="104"/>
       <c r="P78" s="13"/>
       <c r="Q78" s="13"/>
       <c r="R78" s="13"/>
@@ -26156,7 +26210,7 @@
         <v>146</v>
       </c>
       <c r="B79" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C79" s="45" t="s">
         <v>35</v>
@@ -26253,7 +26307,7 @@
         <v>72</v>
       </c>
       <c r="B80" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>43</v>
@@ -26350,7 +26404,7 @@
         <v>73</v>
       </c>
       <c r="B81" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C81" s="15" t="s">
         <v>45</v>
@@ -26447,7 +26501,7 @@
         <v>75</v>
       </c>
       <c r="B82" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>46</v>
@@ -26480,10 +26534,10 @@
         <v>1003</v>
       </c>
       <c r="M82" s="22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N82" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O82" s="22" t="s">
         <v>49</v>
@@ -26543,7 +26597,7 @@
         <v>76</v>
       </c>
       <c r="B83" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>50</v>
@@ -26576,10 +26630,10 @@
         <v>1004</v>
       </c>
       <c r="M83" s="22" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N83" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O83" s="22" t="s">
         <v>49</v>
@@ -26639,7 +26693,7 @@
         <v>77</v>
       </c>
       <c r="B84" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>53</v>
@@ -26675,7 +26729,7 @@
         <v>54</v>
       </c>
       <c r="N84" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O84" s="22" t="s">
         <v>49</v>
@@ -26735,7 +26789,7 @@
         <v>119</v>
       </c>
       <c r="B85" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C85" s="22" t="s">
         <v>55</v>
@@ -26831,7 +26885,7 @@
         <v>78</v>
       </c>
       <c r="B86" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>56</v>
@@ -26867,7 +26921,7 @@
         <v>57</v>
       </c>
       <c r="N86" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O86" s="22" t="s">
         <v>58</v>
@@ -26927,7 +26981,7 @@
         <v>79</v>
       </c>
       <c r="B87" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>59</v>
@@ -26963,7 +27017,7 @@
         <v>60</v>
       </c>
       <c r="N87" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O87" s="22" t="s">
         <v>58</v>
@@ -27023,7 +27077,7 @@
         <v>80</v>
       </c>
       <c r="B88" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>61</v>
@@ -27056,10 +27110,10 @@
         <v>1008</v>
       </c>
       <c r="M88" s="22" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="N88" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O88" s="22" t="s">
         <v>58</v>
@@ -27119,10 +27173,10 @@
         <v>81</v>
       </c>
       <c r="B89" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>36</v>
@@ -27155,7 +27209,7 @@
         <v>64</v>
       </c>
       <c r="N89" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O89" s="22" t="s">
         <v>36</v>
@@ -27215,10 +27269,10 @@
         <v>169</v>
       </c>
       <c r="B90" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="C90" s="51" t="s">
         <v>161</v>
-      </c>
-      <c r="C90" s="51" t="s">
-        <v>165</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>36</v>
@@ -27248,13 +27302,13 @@
         <v>3101</v>
       </c>
       <c r="M90" s="40" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="N90" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O90" s="22" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P90" s="13"/>
       <c r="Q90" s="13"/>
@@ -27312,10 +27366,10 @@
         <v>156</v>
       </c>
       <c r="B91" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C91" s="47" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D91" s="35" t="s">
         <v>36</v>
@@ -27345,13 +27399,13 @@
         <v>3014</v>
       </c>
       <c r="M91" s="47" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N91" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O91" s="58" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="P91" s="13"/>
       <c r="Q91" s="13"/>
@@ -27409,7 +27463,7 @@
         <v>168</v>
       </c>
       <c r="B92" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>98</v>
@@ -27445,7 +27499,7 @@
         <v>99</v>
       </c>
       <c r="N92" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O92" s="22" t="s">
         <v>100</v>
@@ -27456,10 +27510,10 @@
         <v>175</v>
       </c>
       <c r="B93" s="57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D93" s="35" t="s">
         <v>36</v>
@@ -27489,33 +27543,33 @@
         <v>3015</v>
       </c>
       <c r="M93" s="22" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="N93" s="22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="O93" s="22" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:65" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="95" t="s">
-        <v>171</v>
-      </c>
-      <c r="B94" s="96"/>
-      <c r="C94" s="96"/>
-      <c r="D94" s="96"/>
-      <c r="E94" s="96"/>
-      <c r="F94" s="96"/>
-      <c r="G94" s="96"/>
-      <c r="H94" s="96"/>
-      <c r="I94" s="96"/>
-      <c r="J94" s="96"/>
-      <c r="K94" s="96"/>
-      <c r="L94" s="96"/>
-      <c r="M94" s="96"/>
-      <c r="N94" s="96"/>
-      <c r="O94" s="96"/>
+      <c r="A94" s="101" t="s">
+        <v>167</v>
+      </c>
+      <c r="B94" s="102"/>
+      <c r="C94" s="102"/>
+      <c r="D94" s="102"/>
+      <c r="E94" s="102"/>
+      <c r="F94" s="102"/>
+      <c r="G94" s="102"/>
+      <c r="H94" s="102"/>
+      <c r="I94" s="102"/>
+      <c r="J94" s="102"/>
+      <c r="K94" s="102"/>
+      <c r="L94" s="102"/>
+      <c r="M94" s="102"/>
+      <c r="N94" s="102"/>
+      <c r="O94" s="102"/>
       <c r="P94" s="13"/>
       <c r="Q94" s="13"/>
       <c r="R94" s="13"/>
@@ -27568,30 +27622,30 @@
       <c r="BM94" s="13"/>
     </row>
     <row r="95" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="97" t="s">
+      <c r="A95" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B95" s="98"/>
-      <c r="C95" s="98"/>
-      <c r="D95" s="98"/>
-      <c r="E95" s="98"/>
-      <c r="F95" s="98"/>
-      <c r="G95" s="98"/>
-      <c r="H95" s="98"/>
-      <c r="I95" s="98"/>
-      <c r="J95" s="98"/>
-      <c r="K95" s="98"/>
-      <c r="L95" s="98"/>
-      <c r="M95" s="98"/>
-      <c r="N95" s="98"/>
-      <c r="O95" s="98"/>
+      <c r="B95" s="104"/>
+      <c r="C95" s="104"/>
+      <c r="D95" s="104"/>
+      <c r="E95" s="104"/>
+      <c r="F95" s="104"/>
+      <c r="G95" s="104"/>
+      <c r="H95" s="104"/>
+      <c r="I95" s="104"/>
+      <c r="J95" s="104"/>
+      <c r="K95" s="104"/>
+      <c r="L95" s="104"/>
+      <c r="M95" s="104"/>
+      <c r="N95" s="104"/>
+      <c r="O95" s="104"/>
     </row>
     <row r="96" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A96" s="44">
         <v>146</v>
       </c>
       <c r="B96" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C96" s="45" t="s">
         <v>35</v>
@@ -27638,7 +27692,7 @@
         <v>102</v>
       </c>
       <c r="B97" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C97" s="15" t="s">
         <v>43</v>
@@ -27685,7 +27739,7 @@
         <v>103</v>
       </c>
       <c r="B98" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C98" s="15" t="s">
         <v>45</v>
@@ -27732,7 +27786,7 @@
         <v>105</v>
       </c>
       <c r="B99" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C99" s="15" t="s">
         <v>46</v>
@@ -27765,7 +27819,7 @@
         <v>1003</v>
       </c>
       <c r="M99" s="22" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N99" s="22" t="s">
         <v>42</v>
@@ -27779,7 +27833,7 @@
         <v>106</v>
       </c>
       <c r="B100" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>50</v>
@@ -27812,7 +27866,7 @@
         <v>1004</v>
       </c>
       <c r="M100" s="22" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="N100" s="22" t="s">
         <v>42</v>
@@ -27826,7 +27880,7 @@
         <v>121</v>
       </c>
       <c r="B101" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>55</v>
@@ -27873,7 +27927,7 @@
         <v>107</v>
       </c>
       <c r="B102" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C102" s="22" t="s">
         <v>56</v>
@@ -27920,7 +27974,7 @@
         <v>108</v>
       </c>
       <c r="B103" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>59</v>
@@ -27967,7 +28021,7 @@
         <v>109</v>
       </c>
       <c r="B104" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>61</v>
@@ -28000,7 +28054,7 @@
         <v>1008</v>
       </c>
       <c r="M104" s="22" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="N104" s="22" t="s">
         <v>42</v>
@@ -28014,10 +28068,10 @@
         <v>110</v>
       </c>
       <c r="B105" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D105" s="4">
         <v>302</v>
@@ -28047,7 +28101,7 @@
         <v>5001</v>
       </c>
       <c r="M105" s="22" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N105" s="22" t="s">
         <v>42</v>
@@ -28056,15 +28110,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="31.5" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>111</v>
       </c>
       <c r="B106" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D106" s="4">
         <v>302</v>
@@ -28103,12 +28157,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="31.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>17</v>
       </c>
       <c r="B107" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C107" s="15" t="s">
         <v>72</v>
@@ -28144,21 +28198,21 @@
         <v>73</v>
       </c>
       <c r="N107" s="23" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="O107" s="23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="63" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>112</v>
       </c>
       <c r="B108" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D108" s="16">
         <v>305</v>
@@ -28188,24 +28242,24 @@
         <v>3002</v>
       </c>
       <c r="M108" s="23" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="N108" s="23" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="O108" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" ht="47.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>113</v>
       </c>
       <c r="B109" s="57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C109" s="15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D109" s="16" t="s">
         <v>36</v>
@@ -28235,133 +28289,259 @@
         <v>3003</v>
       </c>
       <c r="M109" s="23" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="N109" s="23" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="O109" s="23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="12"/>
-      <c r="B110" s="13"/>
-      <c r="C110" s="52"/>
-      <c r="D110" s="12"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="12"/>
-      <c r="G110" s="27"/>
-      <c r="H110" s="27"/>
-      <c r="I110" s="27"/>
-      <c r="J110" s="12"/>
-      <c r="K110" s="12"/>
-      <c r="L110" s="12"/>
-      <c r="M110" s="13"/>
-      <c r="N110" s="13"/>
-      <c r="O110" s="13"/>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A111" s="12"/>
-      <c r="B111" s="13"/>
-      <c r="C111" s="52"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
-      <c r="G111" s="27"/>
-      <c r="H111" s="27"/>
-      <c r="I111" s="27"/>
-      <c r="J111" s="12"/>
-      <c r="K111" s="12"/>
-      <c r="L111" s="12"/>
-      <c r="M111" s="13"/>
-      <c r="N111" s="13"/>
-      <c r="O111" s="13"/>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A112" s="12"/>
-      <c r="B112" s="13"/>
-      <c r="C112" s="52"/>
-      <c r="D112" s="12"/>
-      <c r="E112" s="12"/>
-      <c r="F112" s="12"/>
-      <c r="G112" s="27"/>
-      <c r="H112" s="27"/>
-      <c r="I112" s="27"/>
-      <c r="J112" s="12"/>
-      <c r="K112" s="12"/>
-      <c r="L112" s="12"/>
-      <c r="M112" s="13"/>
-      <c r="N112" s="13"/>
-      <c r="O112" s="13"/>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A113" s="12"/>
-      <c r="B113" s="13"/>
-      <c r="C113" s="52"/>
-      <c r="D113" s="12"/>
-      <c r="E113" s="12"/>
-      <c r="F113" s="12"/>
-      <c r="G113" s="27"/>
-      <c r="H113" s="27"/>
-      <c r="I113" s="27"/>
-      <c r="J113" s="12"/>
-      <c r="K113" s="12"/>
-      <c r="L113" s="12"/>
-      <c r="M113" s="13"/>
-      <c r="N113" s="13"/>
-      <c r="O113" s="13"/>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="12"/>
-      <c r="B114" s="13"/>
-      <c r="C114" s="52"/>
-      <c r="D114" s="12"/>
-      <c r="E114" s="12"/>
-      <c r="F114" s="12"/>
-      <c r="G114" s="27"/>
-      <c r="H114" s="27"/>
-      <c r="I114" s="27"/>
-      <c r="J114" s="12"/>
-      <c r="K114" s="12"/>
-      <c r="L114" s="12"/>
-      <c r="M114" s="13"/>
-      <c r="N114" s="13"/>
-      <c r="O114" s="13"/>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A115" s="12"/>
-      <c r="B115" s="13"/>
-      <c r="C115" s="52"/>
-      <c r="D115" s="12"/>
-      <c r="E115" s="12"/>
-      <c r="F115" s="12"/>
-      <c r="G115" s="27"/>
-      <c r="H115" s="27"/>
-      <c r="I115" s="27"/>
-      <c r="J115" s="12"/>
-      <c r="K115" s="12"/>
-      <c r="L115" s="12"/>
-      <c r="M115" s="13"/>
-      <c r="N115" s="13"/>
-      <c r="O115" s="13"/>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A116" s="12"/>
-      <c r="B116" s="13"/>
-      <c r="C116" s="52"/>
-      <c r="D116" s="12"/>
-      <c r="E116" s="12"/>
-      <c r="F116" s="12"/>
-      <c r="G116" s="27"/>
-      <c r="H116" s="27"/>
-      <c r="I116" s="27"/>
-      <c r="J116" s="12"/>
-      <c r="K116" s="12"/>
-      <c r="L116" s="12"/>
-      <c r="M116" s="13"/>
-      <c r="N116" s="13"/>
-      <c r="O116" s="13"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="100" t="s">
+        <v>195</v>
+      </c>
+      <c r="B110" s="100"/>
+      <c r="C110" s="100"/>
+      <c r="D110" s="100"/>
+      <c r="E110" s="100"/>
+      <c r="F110" s="100"/>
+      <c r="G110" s="100"/>
+      <c r="H110" s="100"/>
+      <c r="I110" s="100"/>
+      <c r="J110" s="100"/>
+      <c r="K110" s="100"/>
+      <c r="L110" s="100"/>
+      <c r="M110" s="100"/>
+      <c r="N110" s="100"/>
+      <c r="O110" s="100"/>
+    </row>
+    <row r="111" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="97" t="s">
+        <v>200</v>
+      </c>
+      <c r="B111" s="98"/>
+      <c r="C111" s="98"/>
+      <c r="D111" s="98"/>
+      <c r="E111" s="98"/>
+      <c r="F111" s="98"/>
+      <c r="G111" s="98"/>
+      <c r="H111" s="98"/>
+      <c r="I111" s="98"/>
+      <c r="J111" s="98"/>
+      <c r="K111" s="98"/>
+      <c r="L111" s="98"/>
+      <c r="M111" s="98"/>
+      <c r="N111" s="98"/>
+      <c r="O111" s="99"/>
+    </row>
+    <row r="112" spans="1:15" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="4">
+        <v>163</v>
+      </c>
+      <c r="B112" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C112" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="D112" s="4">
+        <v>17</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F112" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G112" s="16">
+        <v>200</v>
+      </c>
+      <c r="H112" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I112" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J112" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K112" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L112" s="5">
+        <v>2603</v>
+      </c>
+      <c r="M112" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="N112" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="O112" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4">
+        <v>164</v>
+      </c>
+      <c r="B113" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C113" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F113" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G113" s="16">
+        <v>200</v>
+      </c>
+      <c r="H113" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I113" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J113" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K113" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L113" s="5">
+        <v>2604</v>
+      </c>
+      <c r="M113" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="N113" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="O113" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="97" t="s">
+        <v>201</v>
+      </c>
+      <c r="B114" s="98"/>
+      <c r="C114" s="98"/>
+      <c r="D114" s="98"/>
+      <c r="E114" s="98"/>
+      <c r="F114" s="98"/>
+      <c r="G114" s="98"/>
+      <c r="H114" s="98"/>
+      <c r="I114" s="98"/>
+      <c r="J114" s="98"/>
+      <c r="K114" s="98"/>
+      <c r="L114" s="98"/>
+      <c r="M114" s="98"/>
+      <c r="N114" s="98"/>
+      <c r="O114" s="99"/>
+    </row>
+    <row r="115" spans="1:15" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="4">
+        <v>163</v>
+      </c>
+      <c r="B115" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C115" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="D115" s="4">
+        <v>17</v>
+      </c>
+      <c r="E115" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F115" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G115" s="16">
+        <v>200</v>
+      </c>
+      <c r="H115" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I115" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J115" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K115" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L115" s="5">
+        <v>2603</v>
+      </c>
+      <c r="M115" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="N115" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="O115" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4">
+        <v>164</v>
+      </c>
+      <c r="B116" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C116" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F116" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G116" s="16">
+        <v>200</v>
+      </c>
+      <c r="H116" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="I116" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J116" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K116" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L116" s="5">
+        <v>2604</v>
+      </c>
+      <c r="M116" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="N116" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="O116" s="22" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" s="12"/>
@@ -32191,6 +32371,7 @@
     <row r="342" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A342" s="12"/>
       <c r="B342" s="13"/>
+      <c r="C342" s="52"/>
       <c r="D342" s="12"/>
       <c r="E342" s="12"/>
       <c r="F342" s="12"/>
@@ -32204,38 +32385,156 @@
       <c r="N342" s="13"/>
       <c r="O342" s="13"/>
     </row>
+    <row r="343" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A343" s="12"/>
+      <c r="B343" s="13"/>
+      <c r="C343" s="52"/>
+      <c r="D343" s="12"/>
+      <c r="E343" s="12"/>
+      <c r="F343" s="12"/>
+      <c r="G343" s="27"/>
+      <c r="H343" s="27"/>
+      <c r="I343" s="27"/>
+      <c r="J343" s="12"/>
+      <c r="K343" s="12"/>
+      <c r="L343" s="12"/>
+      <c r="M343" s="13"/>
+      <c r="N343" s="13"/>
+      <c r="O343" s="13"/>
+    </row>
+    <row r="344" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A344" s="12"/>
+      <c r="B344" s="13"/>
+      <c r="C344" s="52"/>
+      <c r="D344" s="12"/>
+      <c r="E344" s="12"/>
+      <c r="F344" s="12"/>
+      <c r="G344" s="27"/>
+      <c r="H344" s="27"/>
+      <c r="I344" s="27"/>
+      <c r="J344" s="12"/>
+      <c r="K344" s="12"/>
+      <c r="L344" s="12"/>
+      <c r="M344" s="13"/>
+      <c r="N344" s="13"/>
+      <c r="O344" s="13"/>
+    </row>
+    <row r="345" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A345" s="12"/>
+      <c r="B345" s="13"/>
+      <c r="D345" s="12"/>
+      <c r="E345" s="12"/>
+      <c r="F345" s="12"/>
+      <c r="G345" s="27"/>
+      <c r="H345" s="27"/>
+      <c r="I345" s="27"/>
+      <c r="J345" s="12"/>
+      <c r="K345" s="12"/>
+      <c r="L345" s="12"/>
+      <c r="M345" s="13"/>
+      <c r="N345" s="13"/>
+      <c r="O345" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="A77:O77"/>
+    <mergeCell ref="A63:O63"/>
+    <mergeCell ref="A78:O78"/>
     <mergeCell ref="A62:O62"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="A19:O19"/>
     <mergeCell ref="A47:O47"/>
     <mergeCell ref="A48:O48"/>
+    <mergeCell ref="A114:O114"/>
+    <mergeCell ref="A110:O110"/>
+    <mergeCell ref="A111:O111"/>
     <mergeCell ref="A94:O94"/>
     <mergeCell ref="A95:O95"/>
-    <mergeCell ref="A77:O77"/>
-    <mergeCell ref="A63:O63"/>
-    <mergeCell ref="A78:O78"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L57:L61 L11:L15 L72:L76 L23:L24 L31:L32 L17:L18 L7:L9 L68:L70 L53:L55 L26:L29 L86:L89 L103:L108 L82:L84 L99:L101 L92" xr:uid="{8072A8F1-1A15-4450-88CE-A1709A757457}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K57:K61 K72:K76 K68:K70 K7:K9 K53:K55 K11:K18 K23:K45 K82:K84 K103:K109 K99:K101 K86:K93" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K57:K61 K72:K76 K68:K70 K7:K9 K53:K55 K11:K18 K23:K45 K82:K84 K103:K109 K99:K101 K86:K93 K115:K116 K112:K113" xr:uid="{C2076C15-2C9A-460C-AFB6-61CB69F6633F}">
       <formula1>"Field,Cross Field,Cross Form"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J57:J61 J72:J76 J68:J70 J7:J9 J53:J55 J11:J18 J23:J45 J82:J84 J103:J109 J99:J101 J86:J93" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J57:J61 J72:J76 J68:J70 J7:J9 J53:J55 J11:J18 J23:J45 J82:J84 J103:J109 J99:J101 J86:J93 J115:J116 J112:J113" xr:uid="{4FC132A4-15BC-427B-842E-52711B772CED}">
       <formula1>"Error,Warning"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C38" location="ERR_Validation!A110" display="See Appendix A below for allowable amounts for specific years" xr:uid="{3145707C-310F-4C9A-8CC0-DFECAB116321}"/>
+    <hyperlink ref="C39" location="ERR_Validation!A110" display="See Appendix A below for allowable number of submissions for specific years" xr:uid="{A42FA457-322D-4341-9479-FD182D7DF9D9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l29cd52af9b640b690e3347aa75f97a9>
+    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ade64af1c6a24cfdbe8da7f962b31d74>
+    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
+        </TermInfo>
+      </Terms>
+    </e62af2f156934d1aab35222180c5fbb1>
+    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
+        </TermInfo>
+      </Terms>
+    </nb82aa7489a64919aab5fd247ffa0d1e>
+    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
+        </TermInfo>
+      </Terms>
+    </f62107d924a7469492625f91956e46a6>
+    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e9be08524f454d8b979862330e952271>
+    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Value>97</Value>
+      <Value>45</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <UserInfo>
+        <DisplayName>Hunt, Martin</DisplayName>
+        <AccountId>118</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Word document" ma:contentTypeID="0x010100852E11B2A94E4937B655CB4FCD918453006DFD5C59A7CB45AAB5046F3899BB7DEC00F397826DF95DEB4B8DB89BEACF2240F1" ma:contentTypeVersion="79" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="2efa76ee5d5cd602cc18ca32df57176e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9394a98c30c487d0596bd1768260a67a" ns2:_="">
     <xsd:import namespace="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
@@ -32455,68 +32754,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l29cd52af9b640b690e3347aa75f97a9>
-    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ade64af1c6a24cfdbe8da7f962b31d74>
-    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
-        </TermInfo>
-      </Terms>
-    </e62af2f156934d1aab35222180c5fbb1>
-    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
-        </TermInfo>
-      </Terms>
-    </nb82aa7489a64919aab5fd247ffa0d1e>
-    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
-        </TermInfo>
-      </Terms>
-    </f62107d924a7469492625f91956e46a6>
-    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e9be08524f454d8b979862330e952271>
-    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Value>97</Value>
-      <Value>45</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <UserInfo>
-        <DisplayName>Hunt, Martin</DisplayName>
-        <AccountId>118</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8031746-25E9-4E51-ABEB-14F1D0CC1382}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32532,22 +32788,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ERR - updates to validation rules
</commit_message>
<xml_diff>
--- a/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
+++ b/PIT4/validation-rules/Enhanced Reporting Validation Rules.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC44648-4715-4B1E-ABAD-91CA44EA9945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A13FCDF2-C7DA-4519-A352-D504364FF2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Control" sheetId="5" r:id="rId1"/>
@@ -414,9 +414,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>T and S can for site based employees can  not exceed 8716.80 (181.60 x 48). (value may change in future)</t>
-  </si>
-  <si>
     <t>Date can not be before 01/01/24</t>
   </si>
   <si>
@@ -662,6 +659,9 @@
   </si>
   <si>
     <t>176, 177, 178, 179, 180</t>
+  </si>
+  <si>
+    <t>T and S can for site based employees can  not exceed 8720.64 (181.68 x 48). (value may change in future)</t>
   </si>
 </sst>
 </file>
@@ -1308,6 +1308,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1328,6 +1331,18 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1355,21 +1370,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -22037,7 +22037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B8:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22051,18 +22051,18 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
@@ -22103,7 +22103,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="94">
+      <c r="B14" s="95">
         <v>0.12</v>
       </c>
       <c r="C14" s="71">
@@ -22112,59 +22112,59 @@
       <c r="D14" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="97">
+      <c r="E14" s="98">
         <v>45218</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="95"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="34" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="98"/>
+      <c r="E15" s="99"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="95"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="98"/>
+      <c r="E16" s="99"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="95"/>
+      <c r="B17" s="96"/>
       <c r="C17" s="71" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="98"/>
+      <c r="E17" s="99"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="96"/>
+      <c r="B18" s="97"/>
       <c r="C18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="99"/>
+      <c r="E18" s="100"/>
     </row>
     <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="59">
         <v>0.13</v>
       </c>
       <c r="C19" s="71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E19" s="70">
         <v>45272</v>
@@ -22175,10 +22175,10 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="C20" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="34" t="s">
         <v>186</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>187</v>
       </c>
       <c r="E20" s="88">
         <v>45371</v>
@@ -22192,7 +22192,7 @@
         <v>173</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E21" s="70">
         <v>45373</v>
@@ -22206,7 +22206,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E22" s="70">
         <v>45582</v>
@@ -22218,7 +22218,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E23" s="70">
         <v>45582</v>
@@ -22229,10 +22229,10 @@
         <v>0.17</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E24" s="70">
         <v>45635</v>
@@ -22521,7 +22521,9 @@
   </sheetPr>
   <dimension ref="A1:BN350"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -22589,43 +22591,43 @@
       <c r="P1" s="12"/>
     </row>
     <row r="2" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="105"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="110"/>
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="103"/>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="103"/>
-      <c r="L3" s="103"/>
-      <c r="M3" s="103"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="104"/>
+      <c r="B3" s="108"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="109"/>
       <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:65" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -23394,9 +23396,9 @@
         <v>34</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="D19" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="D19" s="93" t="s">
         <v>36</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -23424,7 +23426,7 @@
         <v>1014</v>
       </c>
       <c r="M19" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N19" s="32" t="s">
         <v>36</v>
@@ -23484,23 +23486,23 @@
       <c r="BN19" s="14"/>
     </row>
     <row r="20" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="102" t="s">
+      <c r="A20" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="103"/>
-      <c r="C20" s="103"/>
-      <c r="D20" s="103"/>
-      <c r="E20" s="103"/>
-      <c r="F20" s="103"/>
-      <c r="G20" s="103"/>
-      <c r="H20" s="103"/>
-      <c r="I20" s="103"/>
-      <c r="J20" s="103"/>
-      <c r="K20" s="103"/>
-      <c r="L20" s="103"/>
-      <c r="M20" s="103"/>
-      <c r="N20" s="103"/>
-      <c r="O20" s="104"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="108"/>
+      <c r="K20" s="108"/>
+      <c r="L20" s="108"/>
+      <c r="M20" s="108"/>
+      <c r="N20" s="108"/>
+      <c r="O20" s="109"/>
       <c r="P20" s="13"/>
     </row>
     <row r="21" spans="1:66" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -24360,7 +24362,7 @@
         <v>34</v>
       </c>
       <c r="C39" s="89" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D39" s="4">
         <v>17</v>
@@ -24390,7 +24392,7 @@
         <v>2603</v>
       </c>
       <c r="M39" s="91" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N39" s="22" t="s">
         <v>77</v>
@@ -24407,7 +24409,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="89" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>36</v>
@@ -24437,7 +24439,7 @@
         <v>2604</v>
       </c>
       <c r="M40" s="92" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N40" s="22" t="s">
         <v>77</v>
@@ -24454,7 +24456,7 @@
         <v>34</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>129</v>
+        <v>203</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>36</v>
@@ -24501,7 +24503,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>36</v>
@@ -24531,7 +24533,7 @@
         <v>2606</v>
       </c>
       <c r="M42" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N42" s="22" t="s">
         <v>77</v>
@@ -24548,7 +24550,7 @@
         <v>34</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>36</v>
@@ -24587,7 +24589,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>170</v>
       </c>
@@ -24595,7 +24597,7 @@
         <v>34</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D44" s="4">
         <v>19</v>
@@ -24625,7 +24627,7 @@
         <v>2609</v>
       </c>
       <c r="M44" s="50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N44" s="22" t="s">
         <v>77</v>
@@ -24642,7 +24644,7 @@
         <v>34</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>36</v>
@@ -24672,7 +24674,7 @@
         <v>2610</v>
       </c>
       <c r="M45" s="50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N45" s="22" t="s">
         <v>77</v>
@@ -24689,7 +24691,7 @@
         <v>34</v>
       </c>
       <c r="C46" s="77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D46" s="75" t="s">
         <v>36</v>
@@ -24719,7 +24721,7 @@
         <v>2611</v>
       </c>
       <c r="M46" s="80" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N46" s="81" t="s">
         <v>77</v>
@@ -24736,7 +24738,7 @@
         <v>34</v>
       </c>
       <c r="C47" s="84" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D47" s="82" t="s">
         <v>36</v>
@@ -24766,53 +24768,53 @@
         <v>2614</v>
       </c>
       <c r="M47" s="87" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N47" s="83" t="s">
         <v>77</v>
       </c>
       <c r="O47" s="83" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="106" t="s">
-        <v>139</v>
-      </c>
-      <c r="B48" s="107"/>
-      <c r="C48" s="107"/>
-      <c r="D48" s="107"/>
-      <c r="E48" s="107"/>
-      <c r="F48" s="107"/>
-      <c r="G48" s="107"/>
-      <c r="H48" s="107"/>
-      <c r="I48" s="107"/>
-      <c r="J48" s="107"/>
-      <c r="K48" s="107"/>
-      <c r="L48" s="107"/>
-      <c r="M48" s="107"/>
-      <c r="N48" s="107"/>
-      <c r="O48" s="108"/>
+      <c r="A48" s="111" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="112"/>
+      <c r="C48" s="112"/>
+      <c r="D48" s="112"/>
+      <c r="E48" s="112"/>
+      <c r="F48" s="112"/>
+      <c r="G48" s="112"/>
+      <c r="H48" s="112"/>
+      <c r="I48" s="112"/>
+      <c r="J48" s="112"/>
+      <c r="K48" s="112"/>
+      <c r="L48" s="112"/>
+      <c r="M48" s="112"/>
+      <c r="N48" s="112"/>
+      <c r="O48" s="113"/>
       <c r="P48" s="13"/>
     </row>
     <row r="49" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="102" t="s">
+      <c r="A49" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="103"/>
-      <c r="C49" s="103"/>
-      <c r="D49" s="103"/>
-      <c r="E49" s="103"/>
-      <c r="F49" s="103"/>
-      <c r="G49" s="103"/>
-      <c r="H49" s="103"/>
-      <c r="I49" s="103"/>
-      <c r="J49" s="103"/>
-      <c r="K49" s="103"/>
-      <c r="L49" s="103"/>
-      <c r="M49" s="103"/>
-      <c r="N49" s="103"/>
-      <c r="O49" s="104"/>
+      <c r="B49" s="108"/>
+      <c r="C49" s="108"/>
+      <c r="D49" s="108"/>
+      <c r="E49" s="108"/>
+      <c r="F49" s="108"/>
+      <c r="G49" s="108"/>
+      <c r="H49" s="108"/>
+      <c r="I49" s="108"/>
+      <c r="J49" s="108"/>
+      <c r="K49" s="108"/>
+      <c r="L49" s="108"/>
+      <c r="M49" s="108"/>
+      <c r="N49" s="108"/>
+      <c r="O49" s="109"/>
       <c r="P49" s="13"/>
     </row>
     <row r="50" spans="1:66" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -24820,10 +24822,10 @@
         <v>148</v>
       </c>
       <c r="B50" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="45" t="s">
         <v>140</v>
-      </c>
-      <c r="C50" s="45" t="s">
-        <v>141</v>
       </c>
       <c r="D50" s="44" t="s">
         <v>36</v>
@@ -24853,10 +24855,10 @@
         <v>1111</v>
       </c>
       <c r="M50" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="N50" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="N50" s="22" t="s">
-        <v>143</v>
       </c>
       <c r="O50" s="22" t="s">
         <v>58</v>
@@ -24868,7 +24870,7 @@
         <v>146</v>
       </c>
       <c r="B51" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C51" s="45" t="s">
         <v>35</v>
@@ -24916,7 +24918,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C52" s="23" t="s">
         <v>43</v>
@@ -24964,7 +24966,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>45</v>
@@ -25012,7 +25014,7 @@
         <v>55</v>
       </c>
       <c r="B54" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>46</v>
@@ -25045,10 +25047,10 @@
         <v>1003</v>
       </c>
       <c r="M54" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N54" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O54" s="22" t="s">
         <v>49</v>
@@ -25059,10 +25061,10 @@
         <v>56</v>
       </c>
       <c r="B55" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>36</v>
@@ -25092,10 +25094,10 @@
         <v>1004</v>
       </c>
       <c r="M55" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N55" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O55" s="22" t="s">
         <v>49</v>
@@ -25106,7 +25108,7 @@
         <v>77</v>
       </c>
       <c r="B56" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>53</v>
@@ -25202,7 +25204,7 @@
         <v>117</v>
       </c>
       <c r="B57" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C57" s="22" t="s">
         <v>55</v>
@@ -25249,7 +25251,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>56</v>
@@ -25285,7 +25287,7 @@
         <v>57</v>
       </c>
       <c r="N58" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O58" s="22" t="s">
         <v>58</v>
@@ -25296,7 +25298,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C59" s="15" t="s">
         <v>59</v>
@@ -25332,21 +25334,21 @@
         <v>60</v>
       </c>
       <c r="N59" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O59" s="22" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:66" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:66" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>59</v>
       </c>
       <c r="B60" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>36</v>
@@ -25379,7 +25381,7 @@
         <v>62</v>
       </c>
       <c r="N60" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O60" s="22" t="s">
         <v>58</v>
@@ -25390,7 +25392,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>63</v>
@@ -25426,7 +25428,7 @@
         <v>64</v>
       </c>
       <c r="N61" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O61" s="22" t="s">
         <v>36</v>
@@ -25437,10 +25439,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>36</v>
@@ -25470,7 +25472,7 @@
         <v>2501</v>
       </c>
       <c r="M62" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N62" s="22" t="s">
         <v>67</v>
@@ -25484,12 +25486,12 @@
         <v>177</v>
       </c>
       <c r="B63" s="57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="D63" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="D63" s="93" t="s">
         <v>36</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -25517,7 +25519,7 @@
         <v>1014</v>
       </c>
       <c r="M63" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N63" s="32" t="s">
         <v>36</v>
@@ -25577,43 +25579,43 @@
       <c r="BN63" s="14"/>
     </row>
     <row r="64" spans="1:66" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="100" t="s">
-        <v>150</v>
-      </c>
-      <c r="B64" s="101"/>
-      <c r="C64" s="101"/>
-      <c r="D64" s="101"/>
-      <c r="E64" s="101"/>
-      <c r="F64" s="101"/>
-      <c r="G64" s="101"/>
-      <c r="H64" s="101"/>
-      <c r="I64" s="101"/>
-      <c r="J64" s="101"/>
-      <c r="K64" s="101"/>
-      <c r="L64" s="101"/>
-      <c r="M64" s="101"/>
-      <c r="N64" s="101"/>
-      <c r="O64" s="105"/>
+      <c r="A64" s="105" t="s">
+        <v>149</v>
+      </c>
+      <c r="B64" s="106"/>
+      <c r="C64" s="106"/>
+      <c r="D64" s="106"/>
+      <c r="E64" s="106"/>
+      <c r="F64" s="106"/>
+      <c r="G64" s="106"/>
+      <c r="H64" s="106"/>
+      <c r="I64" s="106"/>
+      <c r="J64" s="106"/>
+      <c r="K64" s="106"/>
+      <c r="L64" s="106"/>
+      <c r="M64" s="106"/>
+      <c r="N64" s="106"/>
+      <c r="O64" s="110"/>
       <c r="P64" s="13"/>
     </row>
     <row r="65" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="102" t="s">
+      <c r="A65" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="B65" s="103"/>
-      <c r="C65" s="103"/>
-      <c r="D65" s="103"/>
-      <c r="E65" s="103"/>
-      <c r="F65" s="103"/>
-      <c r="G65" s="103"/>
-      <c r="H65" s="103"/>
-      <c r="I65" s="103"/>
-      <c r="J65" s="103"/>
-      <c r="K65" s="103"/>
-      <c r="L65" s="103"/>
-      <c r="M65" s="103"/>
-      <c r="N65" s="103"/>
-      <c r="O65" s="104"/>
+      <c r="B65" s="108"/>
+      <c r="C65" s="108"/>
+      <c r="D65" s="108"/>
+      <c r="E65" s="108"/>
+      <c r="F65" s="108"/>
+      <c r="G65" s="108"/>
+      <c r="H65" s="108"/>
+      <c r="I65" s="108"/>
+      <c r="J65" s="108"/>
+      <c r="K65" s="108"/>
+      <c r="L65" s="108"/>
+      <c r="M65" s="108"/>
+      <c r="N65" s="108"/>
+      <c r="O65" s="109"/>
       <c r="P65" s="13"/>
     </row>
     <row r="66" spans="1:66" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -25621,10 +25623,10 @@
         <v>148</v>
       </c>
       <c r="B66" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C66" s="45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D66" s="44" t="s">
         <v>36</v>
@@ -25654,10 +25656,10 @@
         <v>1111</v>
       </c>
       <c r="M66" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="N66" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="N66" s="22" t="s">
-        <v>143</v>
       </c>
       <c r="O66" s="22" t="s">
         <v>58</v>
@@ -25669,7 +25671,7 @@
         <v>146</v>
       </c>
       <c r="B67" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C67" s="45" t="s">
         <v>35</v>
@@ -25717,7 +25719,7 @@
         <v>62</v>
       </c>
       <c r="B68" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>43</v>
@@ -25765,7 +25767,7 @@
         <v>63</v>
       </c>
       <c r="B69" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C69" s="15" t="s">
         <v>45</v>
@@ -25813,7 +25815,7 @@
         <v>65</v>
       </c>
       <c r="B70" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C70" s="15" t="s">
         <v>46</v>
@@ -25849,7 +25851,7 @@
         <v>48</v>
       </c>
       <c r="N70" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O70" s="4" t="s">
         <v>49</v>
@@ -25860,10 +25862,10 @@
         <v>66</v>
       </c>
       <c r="B71" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>36</v>
@@ -25896,7 +25898,7 @@
         <v>52</v>
       </c>
       <c r="N71" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O71" s="22" t="s">
         <v>49</v>
@@ -25907,7 +25909,7 @@
         <v>77</v>
       </c>
       <c r="B72" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>53</v>
@@ -26003,7 +26005,7 @@
         <v>118</v>
       </c>
       <c r="B73" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C73" s="22" t="s">
         <v>55</v>
@@ -26050,7 +26052,7 @@
         <v>67</v>
       </c>
       <c r="B74" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C74" s="15" t="s">
         <v>56</v>
@@ -26086,7 +26088,7 @@
         <v>57</v>
       </c>
       <c r="N74" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O74" s="22" t="s">
         <v>58</v>
@@ -26097,7 +26099,7 @@
         <v>68</v>
       </c>
       <c r="B75" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>59</v>
@@ -26133,7 +26135,7 @@
         <v>60</v>
       </c>
       <c r="N75" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O75" s="22" t="s">
         <v>58</v>
@@ -26144,7 +26146,7 @@
         <v>69</v>
       </c>
       <c r="B76" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>61</v>
@@ -26177,10 +26179,10 @@
         <v>1008</v>
       </c>
       <c r="M76" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N76" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O76" s="22" t="s">
         <v>58</v>
@@ -26191,7 +26193,7 @@
         <v>70</v>
       </c>
       <c r="B77" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>63</v>
@@ -26227,7 +26229,7 @@
         <v>64</v>
       </c>
       <c r="N77" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O77" s="22" t="s">
         <v>36</v>
@@ -26238,10 +26240,10 @@
         <v>71</v>
       </c>
       <c r="B78" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>36</v>
@@ -26271,13 +26273,13 @@
         <v>2506</v>
       </c>
       <c r="M78" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="N78" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="O78" s="22" t="s">
         <v>154</v>
-      </c>
-      <c r="N78" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="O78" s="22" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
@@ -26285,12 +26287,12 @@
         <v>178</v>
       </c>
       <c r="B79" s="57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C79" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="D79" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="D79" s="93" t="s">
         <v>36</v>
       </c>
       <c r="E79" s="5" t="s">
@@ -26318,7 +26320,7 @@
         <v>1014</v>
       </c>
       <c r="M79" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N79" s="32" t="s">
         <v>36</v>
@@ -26378,23 +26380,23 @@
       <c r="BN79" s="14"/>
     </row>
     <row r="80" spans="1:66" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="100" t="s">
-        <v>156</v>
-      </c>
-      <c r="B80" s="101"/>
-      <c r="C80" s="101"/>
-      <c r="D80" s="101"/>
-      <c r="E80" s="101"/>
-      <c r="F80" s="101"/>
-      <c r="G80" s="101"/>
-      <c r="H80" s="101"/>
-      <c r="I80" s="101"/>
-      <c r="J80" s="101"/>
-      <c r="K80" s="101"/>
-      <c r="L80" s="101"/>
-      <c r="M80" s="101"/>
-      <c r="N80" s="101"/>
-      <c r="O80" s="101"/>
+      <c r="A80" s="105" t="s">
+        <v>155</v>
+      </c>
+      <c r="B80" s="106"/>
+      <c r="C80" s="106"/>
+      <c r="D80" s="106"/>
+      <c r="E80" s="106"/>
+      <c r="F80" s="106"/>
+      <c r="G80" s="106"/>
+      <c r="H80" s="106"/>
+      <c r="I80" s="106"/>
+      <c r="J80" s="106"/>
+      <c r="K80" s="106"/>
+      <c r="L80" s="106"/>
+      <c r="M80" s="106"/>
+      <c r="N80" s="106"/>
+      <c r="O80" s="106"/>
       <c r="P80" s="13"/>
       <c r="Q80" s="13"/>
       <c r="R80" s="13"/>
@@ -26447,23 +26449,23 @@
       <c r="BM80" s="13"/>
     </row>
     <row r="81" spans="1:65" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="102" t="s">
+      <c r="A81" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="B81" s="103"/>
-      <c r="C81" s="103"/>
-      <c r="D81" s="103"/>
-      <c r="E81" s="103"/>
-      <c r="F81" s="103"/>
-      <c r="G81" s="103"/>
-      <c r="H81" s="103"/>
-      <c r="I81" s="103"/>
-      <c r="J81" s="103"/>
-      <c r="K81" s="103"/>
-      <c r="L81" s="103"/>
-      <c r="M81" s="103"/>
-      <c r="N81" s="103"/>
-      <c r="O81" s="103"/>
+      <c r="B81" s="108"/>
+      <c r="C81" s="108"/>
+      <c r="D81" s="108"/>
+      <c r="E81" s="108"/>
+      <c r="F81" s="108"/>
+      <c r="G81" s="108"/>
+      <c r="H81" s="108"/>
+      <c r="I81" s="108"/>
+      <c r="J81" s="108"/>
+      <c r="K81" s="108"/>
+      <c r="L81" s="108"/>
+      <c r="M81" s="108"/>
+      <c r="N81" s="108"/>
+      <c r="O81" s="108"/>
       <c r="P81" s="13"/>
       <c r="Q81" s="13"/>
       <c r="R81" s="13"/>
@@ -26520,7 +26522,7 @@
         <v>146</v>
       </c>
       <c r="B82" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C82" s="45" t="s">
         <v>35</v>
@@ -26617,7 +26619,7 @@
         <v>72</v>
       </c>
       <c r="B83" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C83" s="15" t="s">
         <v>43</v>
@@ -26714,7 +26716,7 @@
         <v>73</v>
       </c>
       <c r="B84" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>45</v>
@@ -26811,7 +26813,7 @@
         <v>75</v>
       </c>
       <c r="B85" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>46</v>
@@ -26844,10 +26846,10 @@
         <v>1003</v>
       </c>
       <c r="M85" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N85" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O85" s="22" t="s">
         <v>49</v>
@@ -26902,12 +26904,12 @@
       <c r="BL85" s="14"/>
       <c r="BM85" s="14"/>
     </row>
-    <row r="86" spans="1:65" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:65" ht="63" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>76</v>
       </c>
       <c r="B86" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>50</v>
@@ -26940,10 +26942,10 @@
         <v>1004</v>
       </c>
       <c r="M86" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N86" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O86" s="22" t="s">
         <v>49</v>
@@ -27003,7 +27005,7 @@
         <v>77</v>
       </c>
       <c r="B87" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>53</v>
@@ -27039,7 +27041,7 @@
         <v>54</v>
       </c>
       <c r="N87" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O87" s="22" t="s">
         <v>49</v>
@@ -27099,7 +27101,7 @@
         <v>119</v>
       </c>
       <c r="B88" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C88" s="22" t="s">
         <v>55</v>
@@ -27195,7 +27197,7 @@
         <v>78</v>
       </c>
       <c r="B89" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>56</v>
@@ -27231,7 +27233,7 @@
         <v>57</v>
       </c>
       <c r="N89" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O89" s="22" t="s">
         <v>58</v>
@@ -27291,7 +27293,7 @@
         <v>79</v>
       </c>
       <c r="B90" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>59</v>
@@ -27327,7 +27329,7 @@
         <v>60</v>
       </c>
       <c r="N90" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O90" s="22" t="s">
         <v>58</v>
@@ -27387,7 +27389,7 @@
         <v>80</v>
       </c>
       <c r="B91" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>61</v>
@@ -27420,10 +27422,10 @@
         <v>1008</v>
       </c>
       <c r="M91" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N91" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O91" s="22" t="s">
         <v>58</v>
@@ -27483,10 +27485,10 @@
         <v>81</v>
       </c>
       <c r="B92" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>36</v>
@@ -27519,7 +27521,7 @@
         <v>64</v>
       </c>
       <c r="N92" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O92" s="22" t="s">
         <v>36</v>
@@ -27579,10 +27581,10 @@
         <v>169</v>
       </c>
       <c r="B93" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C93" s="51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>36</v>
@@ -27612,13 +27614,13 @@
         <v>3101</v>
       </c>
       <c r="M93" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="N93" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="O93" s="22" t="s">
         <v>162</v>
-      </c>
-      <c r="N93" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="O93" s="22" t="s">
-        <v>163</v>
       </c>
       <c r="P93" s="13"/>
       <c r="Q93" s="13"/>
@@ -27676,10 +27678,10 @@
         <v>156</v>
       </c>
       <c r="B94" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C94" s="47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D94" s="35" t="s">
         <v>36</v>
@@ -27709,13 +27711,13 @@
         <v>3014</v>
       </c>
       <c r="M94" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="N94" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="O94" s="58" t="s">
         <v>165</v>
-      </c>
-      <c r="N94" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="O94" s="58" t="s">
-        <v>166</v>
       </c>
       <c r="P94" s="13"/>
       <c r="Q94" s="13"/>
@@ -27773,7 +27775,7 @@
         <v>168</v>
       </c>
       <c r="B95" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>98</v>
@@ -27809,7 +27811,7 @@
         <v>99</v>
       </c>
       <c r="N95" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O95" s="22" t="s">
         <v>100</v>
@@ -27820,10 +27822,10 @@
         <v>175</v>
       </c>
       <c r="B96" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D96" s="35" t="s">
         <v>36</v>
@@ -27853,13 +27855,13 @@
         <v>3015</v>
       </c>
       <c r="M96" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N96" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O96" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="97" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
@@ -27867,12 +27869,12 @@
         <v>179</v>
       </c>
       <c r="B97" s="57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C97" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="D97" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="D97" s="93" t="s">
         <v>36</v>
       </c>
       <c r="E97" s="5" t="s">
@@ -27900,7 +27902,7 @@
         <v>1014</v>
       </c>
       <c r="M97" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N97" s="32" t="s">
         <v>36</v>
@@ -27960,23 +27962,23 @@
       <c r="BN97" s="14"/>
     </row>
     <row r="98" spans="1:66" s="6" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="100" t="s">
-        <v>167</v>
-      </c>
-      <c r="B98" s="101"/>
-      <c r="C98" s="101"/>
-      <c r="D98" s="101"/>
-      <c r="E98" s="101"/>
-      <c r="F98" s="101"/>
-      <c r="G98" s="101"/>
-      <c r="H98" s="101"/>
-      <c r="I98" s="101"/>
-      <c r="J98" s="101"/>
-      <c r="K98" s="101"/>
-      <c r="L98" s="101"/>
-      <c r="M98" s="101"/>
-      <c r="N98" s="101"/>
-      <c r="O98" s="101"/>
+      <c r="A98" s="105" t="s">
+        <v>166</v>
+      </c>
+      <c r="B98" s="106"/>
+      <c r="C98" s="106"/>
+      <c r="D98" s="106"/>
+      <c r="E98" s="106"/>
+      <c r="F98" s="106"/>
+      <c r="G98" s="106"/>
+      <c r="H98" s="106"/>
+      <c r="I98" s="106"/>
+      <c r="J98" s="106"/>
+      <c r="K98" s="106"/>
+      <c r="L98" s="106"/>
+      <c r="M98" s="106"/>
+      <c r="N98" s="106"/>
+      <c r="O98" s="106"/>
       <c r="P98" s="13"/>
       <c r="Q98" s="13"/>
       <c r="R98" s="13"/>
@@ -28029,30 +28031,30 @@
       <c r="BM98" s="13"/>
     </row>
     <row r="99" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="102" t="s">
+      <c r="A99" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="B99" s="103"/>
-      <c r="C99" s="103"/>
-      <c r="D99" s="103"/>
-      <c r="E99" s="103"/>
-      <c r="F99" s="103"/>
-      <c r="G99" s="103"/>
-      <c r="H99" s="103"/>
-      <c r="I99" s="103"/>
-      <c r="J99" s="103"/>
-      <c r="K99" s="103"/>
-      <c r="L99" s="103"/>
-      <c r="M99" s="103"/>
-      <c r="N99" s="103"/>
-      <c r="O99" s="103"/>
+      <c r="B99" s="108"/>
+      <c r="C99" s="108"/>
+      <c r="D99" s="108"/>
+      <c r="E99" s="108"/>
+      <c r="F99" s="108"/>
+      <c r="G99" s="108"/>
+      <c r="H99" s="108"/>
+      <c r="I99" s="108"/>
+      <c r="J99" s="108"/>
+      <c r="K99" s="108"/>
+      <c r="L99" s="108"/>
+      <c r="M99" s="108"/>
+      <c r="N99" s="108"/>
+      <c r="O99" s="108"/>
     </row>
     <row r="100" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A100" s="44">
         <v>146</v>
       </c>
       <c r="B100" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C100" s="45" t="s">
         <v>35</v>
@@ -28099,7 +28101,7 @@
         <v>102</v>
       </c>
       <c r="B101" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C101" s="15" t="s">
         <v>43</v>
@@ -28146,7 +28148,7 @@
         <v>103</v>
       </c>
       <c r="B102" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C102" s="15" t="s">
         <v>45</v>
@@ -28193,7 +28195,7 @@
         <v>105</v>
       </c>
       <c r="B103" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C103" s="15" t="s">
         <v>46</v>
@@ -28226,7 +28228,7 @@
         <v>1003</v>
       </c>
       <c r="M103" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N103" s="22" t="s">
         <v>42</v>
@@ -28235,12 +28237,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="104" spans="1:66" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:66" ht="63" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>106</v>
       </c>
       <c r="B104" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>50</v>
@@ -28273,7 +28275,7 @@
         <v>1004</v>
       </c>
       <c r="M104" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N104" s="22" t="s">
         <v>42</v>
@@ -28287,7 +28289,7 @@
         <v>121</v>
       </c>
       <c r="B105" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>55</v>
@@ -28334,7 +28336,7 @@
         <v>107</v>
       </c>
       <c r="B106" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C106" s="22" t="s">
         <v>56</v>
@@ -28381,7 +28383,7 @@
         <v>108</v>
       </c>
       <c r="B107" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>59</v>
@@ -28428,7 +28430,7 @@
         <v>109</v>
       </c>
       <c r="B108" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>61</v>
@@ -28461,7 +28463,7 @@
         <v>1008</v>
       </c>
       <c r="M108" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N108" s="22" t="s">
         <v>42</v>
@@ -28475,10 +28477,10 @@
         <v>110</v>
       </c>
       <c r="B109" s="57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="D109" s="4">
         <v>302</v>
@@ -28508,7 +28510,7 @@
         <v>5001</v>
       </c>
       <c r="M109" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N109" s="22" t="s">
         <v>42</v>
@@ -28522,10 +28524,10 @@
         <v>111</v>
       </c>
       <c r="B110" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D110" s="4">
         <v>302</v>
@@ -28569,7 +28571,7 @@
         <v>17</v>
       </c>
       <c r="B111" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C111" s="15" t="s">
         <v>72</v>
@@ -28605,7 +28607,7 @@
         <v>73</v>
       </c>
       <c r="N111" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O111" s="23" t="s">
         <v>74</v>
@@ -28616,10 +28618,10 @@
         <v>112</v>
       </c>
       <c r="B112" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D112" s="16">
         <v>305</v>
@@ -28649,13 +28651,13 @@
         <v>3002</v>
       </c>
       <c r="M112" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="N112" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="O112" s="23" t="s">
         <v>174</v>
-      </c>
-      <c r="N112" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="O112" s="23" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:66" ht="47.25" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -28663,10 +28665,10 @@
         <v>113</v>
       </c>
       <c r="B113" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D113" s="16" t="s">
         <v>36</v>
@@ -28696,13 +28698,13 @@
         <v>3003</v>
       </c>
       <c r="M113" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N113" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O113" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="1:66" ht="31.5" x14ac:dyDescent="0.25">
@@ -28710,12 +28712,12 @@
         <v>180</v>
       </c>
       <c r="B114" s="57" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C114" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="D114" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="D114" s="93" t="s">
         <v>36</v>
       </c>
       <c r="E114" s="5" t="s">
@@ -28743,7 +28745,7 @@
         <v>1014</v>
       </c>
       <c r="M114" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N114" s="32" t="s">
         <v>36</v>
@@ -28803,42 +28805,42 @@
       <c r="BN114" s="14"/>
     </row>
     <row r="115" spans="1:66" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A115" s="112" t="s">
-        <v>195</v>
-      </c>
-      <c r="B115" s="112"/>
-      <c r="C115" s="112"/>
-      <c r="D115" s="112"/>
-      <c r="E115" s="112"/>
-      <c r="F115" s="112"/>
-      <c r="G115" s="112"/>
-      <c r="H115" s="112"/>
-      <c r="I115" s="112"/>
-      <c r="J115" s="112"/>
-      <c r="K115" s="112"/>
-      <c r="L115" s="112"/>
-      <c r="M115" s="112"/>
-      <c r="N115" s="112"/>
-      <c r="O115" s="112"/>
+      <c r="A115" s="104" t="s">
+        <v>194</v>
+      </c>
+      <c r="B115" s="104"/>
+      <c r="C115" s="104"/>
+      <c r="D115" s="104"/>
+      <c r="E115" s="104"/>
+      <c r="F115" s="104"/>
+      <c r="G115" s="104"/>
+      <c r="H115" s="104"/>
+      <c r="I115" s="104"/>
+      <c r="J115" s="104"/>
+      <c r="K115" s="104"/>
+      <c r="L115" s="104"/>
+      <c r="M115" s="104"/>
+      <c r="N115" s="104"/>
+      <c r="O115" s="104"/>
     </row>
     <row r="116" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="109" t="s">
-        <v>200</v>
-      </c>
-      <c r="B116" s="110"/>
-      <c r="C116" s="110"/>
-      <c r="D116" s="110"/>
-      <c r="E116" s="110"/>
-      <c r="F116" s="110"/>
-      <c r="G116" s="110"/>
-      <c r="H116" s="110"/>
-      <c r="I116" s="110"/>
-      <c r="J116" s="110"/>
-      <c r="K116" s="110"/>
-      <c r="L116" s="110"/>
-      <c r="M116" s="110"/>
-      <c r="N116" s="110"/>
-      <c r="O116" s="111"/>
+      <c r="A116" s="101" t="s">
+        <v>199</v>
+      </c>
+      <c r="B116" s="102"/>
+      <c r="C116" s="102"/>
+      <c r="D116" s="102"/>
+      <c r="E116" s="102"/>
+      <c r="F116" s="102"/>
+      <c r="G116" s="102"/>
+      <c r="H116" s="102"/>
+      <c r="I116" s="102"/>
+      <c r="J116" s="102"/>
+      <c r="K116" s="102"/>
+      <c r="L116" s="102"/>
+      <c r="M116" s="102"/>
+      <c r="N116" s="102"/>
+      <c r="O116" s="103"/>
     </row>
     <row r="117" spans="1:66" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
@@ -28848,7 +28850,7 @@
         <v>34</v>
       </c>
       <c r="C117" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D117" s="4">
         <v>17</v>
@@ -28878,7 +28880,7 @@
         <v>2603</v>
       </c>
       <c r="M117" s="43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N117" s="22" t="s">
         <v>77</v>
@@ -28895,7 +28897,7 @@
         <v>34</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D118" s="4" t="s">
         <v>36</v>
@@ -28925,7 +28927,7 @@
         <v>2604</v>
       </c>
       <c r="M118" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N118" s="22" t="s">
         <v>77</v>
@@ -28935,23 +28937,23 @@
       </c>
     </row>
     <row r="119" spans="1:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="109" t="s">
-        <v>201</v>
-      </c>
-      <c r="B119" s="110"/>
-      <c r="C119" s="110"/>
-      <c r="D119" s="110"/>
-      <c r="E119" s="110"/>
-      <c r="F119" s="110"/>
-      <c r="G119" s="110"/>
-      <c r="H119" s="110"/>
-      <c r="I119" s="110"/>
-      <c r="J119" s="110"/>
-      <c r="K119" s="110"/>
-      <c r="L119" s="110"/>
-      <c r="M119" s="110"/>
-      <c r="N119" s="110"/>
-      <c r="O119" s="111"/>
+      <c r="A119" s="101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B119" s="102"/>
+      <c r="C119" s="102"/>
+      <c r="D119" s="102"/>
+      <c r="E119" s="102"/>
+      <c r="F119" s="102"/>
+      <c r="G119" s="102"/>
+      <c r="H119" s="102"/>
+      <c r="I119" s="102"/>
+      <c r="J119" s="102"/>
+      <c r="K119" s="102"/>
+      <c r="L119" s="102"/>
+      <c r="M119" s="102"/>
+      <c r="N119" s="102"/>
+      <c r="O119" s="103"/>
     </row>
     <row r="120" spans="1:66" ht="31.5" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
@@ -28961,7 +28963,7 @@
         <v>34</v>
       </c>
       <c r="C120" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D120" s="4">
         <v>17</v>
@@ -28991,7 +28993,7 @@
         <v>2603</v>
       </c>
       <c r="M120" s="43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N120" s="22" t="s">
         <v>77</v>
@@ -29008,7 +29010,7 @@
         <v>34</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D121" s="4" t="s">
         <v>36</v>
@@ -29038,7 +29040,7 @@
         <v>2604</v>
       </c>
       <c r="M121" s="50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N121" s="22" t="s">
         <v>77</v>
@@ -32941,11 +32943,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A119:O119"/>
-    <mergeCell ref="A115:O115"/>
-    <mergeCell ref="A116:O116"/>
-    <mergeCell ref="A98:O98"/>
-    <mergeCell ref="A99:O99"/>
     <mergeCell ref="A80:O80"/>
     <mergeCell ref="A65:O65"/>
     <mergeCell ref="A81:O81"/>
@@ -32955,6 +32952,11 @@
     <mergeCell ref="A20:O20"/>
     <mergeCell ref="A48:O48"/>
     <mergeCell ref="A49:O49"/>
+    <mergeCell ref="A119:O119"/>
+    <mergeCell ref="A115:O115"/>
+    <mergeCell ref="A116:O116"/>
+    <mergeCell ref="A98:O98"/>
+    <mergeCell ref="A99:O99"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <dataValidations count="3">
@@ -32978,12 +32980,55 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l29cd52af9b640b690e3347aa75f97a9>
+    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ade64af1c6a24cfdbe8da7f962b31d74>
+    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
+        </TermInfo>
+      </Terms>
+    </e62af2f156934d1aab35222180c5fbb1>
+    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
+        </TermInfo>
+      </Terms>
+    </nb82aa7489a64919aab5fd247ffa0d1e>
+    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
+        </TermInfo>
+      </Terms>
+    </f62107d924a7469492625f91956e46a6>
+    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </e9be08524f454d8b979862330e952271>
+    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <Value>97</Value>
+      <Value>45</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
+      <UserInfo>
+        <DisplayName>Hunt, Martin</DisplayName>
+        <AccountId>118</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33207,61 +33252,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <l29cd52af9b640b690e3347aa75f97a9 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l29cd52af9b640b690e3347aa75f97a9>
-    <ade64af1c6a24cfdbe8da7f962b31d74 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ade64af1c6a24cfdbe8da7f962b31d74>
-    <e62af2f156934d1aab35222180c5fbb1 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Project Site</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">7b0ab4a9-6be8-4c6c-983c-945fdef69f95</TermId>
-        </TermInfo>
-      </Terms>
-    </e62af2f156934d1aab35222180c5fbb1>
-    <nb82aa7489a64919aab5fd247ffa0d1e xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Enhanced Reporting Requirements</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">b99d9e68-488f-45bf-a303-a86e26269b90</TermId>
-        </TermInfo>
-      </Terms>
-    </nb82aa7489a64919aab5fd247ffa0d1e>
-    <f62107d924a7469492625f91956e46a6 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Development</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">bc803685-9f6b-4a9c-85fc-59591d8af7f6</TermId>
-        </TermInfo>
-      </Terms>
-    </f62107d924a7469492625f91956e46a6>
-    <e9be08524f454d8b979862330e952271 xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </e9be08524f454d8b979862330e952271>
-    <TaxCatchAll xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <Value>97</Value>
-      <Value>45</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <SharedWithUsers xmlns="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8">
-      <UserInfo>
-        <DisplayName>Hunt, Martin</DisplayName>
-        <AccountId>118</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -33285,11 +33289,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87B9136B-9C67-4E28-A05B-CA9673C4F673}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2AB05A4-ABA0-46C7-B81D-486560E213A2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="184185d0-04c6-4ef5-ba23-3d0ec5a17fb8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>